<commit_message>
Update RS01SLBS Cal Sheets
Updates to RS01SLBS_00002.
Updates to RS01SLBS_00003.
</commit_message>
<xml_diff>
--- a/RS01SLBS/Omaha_Cal_Info_RS01SLBS_00002.xlsx
+++ b/RS01SLBS/Omaha_Cal_Info_RS01SLBS_00002.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20160" windowHeight="9615" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20160" windowHeight="9615"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="2" r:id="rId1"/>
@@ -12,12 +12,12 @@
     <sheet name="204_CC_tcarray" sheetId="3" r:id="rId3"/>
     <sheet name="204_CC_taarray" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="66">
   <si>
     <t>Ref Des</t>
   </si>
@@ -215,17 +215,20 @@
   <si>
     <t>[400.10000000, 403.40000000, 406.90000000, 410.30000000, 413.20000000, 416.90000000, 420.60000000, 425.10000000, 429.00000000, 432.90000000, 436.80000000, 440.50000000, 444.70000000, 449.70000000, 453.90000000, 458.20000000, 462.20000000, 466.40000000, 471.10000000, 476.10000000, 480.80000000, 485.50000000, 489.70000000, 494.10000000, 498.10000000, 502.40000000, 506.90000000, 512.10000000, 516.60000000, 521.60000000, 525.60000000, 530.30000000, 534.20000000, 538.50000000, 542.80000000, 547.30000000, 551.20000000, 556.20000000, 560.30000000, 564.90000000, 569.00000000, 572.90000000, 576.60000000, 580.50000000, 584.40000000, 588.50000000, 592.70000000, 597.20000000, 601.80000000, 606.30000000, 610.70000000, 615.40000000, 619.40000000, 623.90000000, 627.50000000, 631.90000000, 635.80000000, 640.00000000, 644.10000000, 648.40000000, 652.50000000, 657.00000000, 661.10000000, 665.40000000, 669.60000000, 674.00000000, 677.80000000, 681.90000000, 685.50000000, 689.00000000, 692.80000000, 696.30000000, 699.90000000, 703.30000000, 707.00000000, 710.00000000, 713.60000000, 717.10000000, 720.00000000, 723.70000000, 726.50000000, 729.90000000, 732.30000000]</t>
   </si>
+  <si>
+    <t>TN-313</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="#,##0.000000000"/>
     <numFmt numFmtId="165" formatCode="hh:mm:ss\ AM/PM"/>
     <numFmt numFmtId="166" formatCode="#,##0.00000"/>
   </numFmts>
-  <fonts count="35" x14ac:knownFonts="1">
+  <fonts count="35">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1259,7 +1262,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1294,7 +1296,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1470,14 +1471,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z231"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="21.28515625" customWidth="1"/>
     <col min="4" max="4" width="22.28515625" customWidth="1"/>
@@ -1486,7 +1487,7 @@
     <col min="14" max="14" width="49" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="15.75" customHeight="1">
       <c r="A1" s="56" t="s">
         <v>0</v>
       </c>
@@ -1536,7 +1537,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" s="45" customFormat="1" ht="15.75" customHeight="1">
       <c r="A2" s="54" t="s">
         <v>27</v>
       </c>
@@ -1563,7 +1564,7 @@
         <v>2921</v>
       </c>
       <c r="J2" s="103" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="K2" s="54"/>
       <c r="L2" s="64">
@@ -1590,7 +1591,7 @@
       <c r="Y2" s="46"/>
       <c r="Z2" s="46"/>
     </row>
-    <row r="3" spans="1:26" s="58" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" s="58" customFormat="1" ht="15.75" customHeight="1">
       <c r="A3" s="54" t="s">
         <v>44</v>
       </c>
@@ -1642,7 +1643,7 @@
       <c r="Y3" s="54"/>
       <c r="Z3" s="54"/>
     </row>
-    <row r="4" spans="1:26" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" s="45" customFormat="1" ht="15.75" customHeight="1">
       <c r="A4" s="59"/>
       <c r="B4" s="59"/>
       <c r="C4" s="60"/>
@@ -1657,7 +1658,7 @@
       <c r="L4" s="58"/>
       <c r="M4" s="58"/>
     </row>
-    <row r="5" spans="1:26" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" s="45" customFormat="1" ht="15.75" customHeight="1">
       <c r="A5" s="52"/>
       <c r="B5" s="52"/>
       <c r="C5" s="48"/>
@@ -1669,7 +1670,7 @@
       <c r="I5" s="51"/>
       <c r="J5" s="51"/>
     </row>
-    <row r="6" spans="1:26" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:26" s="45" customFormat="1" ht="15.75" customHeight="1">
       <c r="A6" s="52"/>
       <c r="B6" s="52"/>
       <c r="C6" s="48"/>
@@ -1681,7 +1682,7 @@
       <c r="I6" s="51"/>
       <c r="J6" s="51"/>
     </row>
-    <row r="7" spans="1:26" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:26" s="45" customFormat="1" ht="15.75" customHeight="1">
       <c r="A7" s="52"/>
       <c r="B7" s="52"/>
       <c r="C7" s="48"/>
@@ -1693,7 +1694,7 @@
       <c r="I7" s="51"/>
       <c r="J7" s="51"/>
     </row>
-    <row r="8" spans="1:26" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:26" s="45" customFormat="1" ht="15.75" customHeight="1">
       <c r="A8" s="52"/>
       <c r="B8" s="52"/>
       <c r="C8" s="48"/>
@@ -1705,239 +1706,239 @@
       <c r="I8" s="51"/>
       <c r="J8" s="51"/>
     </row>
-    <row r="9" spans="1:26" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:26" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:26" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="10" spans="1:26" s="45" customFormat="1" ht="15.75" customHeight="1">
       <c r="A10" s="47"/>
     </row>
-    <row r="11" spans="1:26" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:26" s="45" customFormat="1" ht="15.75" customHeight="1">
       <c r="A11" s="52"/>
     </row>
-    <row r="12" spans="1:26" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:26" s="45" customFormat="1" ht="15.75" customHeight="1">
       <c r="A12" s="47"/>
     </row>
-    <row r="13" spans="1:26" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:26" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:26" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:26" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="14" spans="1:26" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="15" spans="1:26" s="45" customFormat="1" ht="15.75" customHeight="1">
       <c r="G15" s="53" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:26" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="17" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="18" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="19" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="20" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="21" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="23" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="33" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="34" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="35" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="36" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="37" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="38" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="39" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="40" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="41" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="42" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="43" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="44" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="45" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="46" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="47" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="48" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="49" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="50" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="51" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="52" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="53" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="54" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="55" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="56" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="57" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="58" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="59" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="60" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="61" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="62" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="63" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="64" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="65" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="66" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="67" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="68" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="69" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="70" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="71" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="72" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="73" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="74" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="75" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="76" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="77" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="78" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="79" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="80" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="81" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="82" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="83" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="84" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="85" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="86" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="87" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="88" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="89" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="90" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="91" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="92" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="93" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="94" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="95" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="96" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="97" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="98" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="99" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="100" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="101" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="102" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="103" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="104" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="105" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="106" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="107" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="108" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="109" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="110" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="111" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="112" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="113" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="114" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="115" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="116" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="117" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="118" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="119" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="120" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="121" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="122" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="123" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="124" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="125" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="126" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="127" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="128" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="129" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="130" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="131" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="132" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="133" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="134" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="135" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="136" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="137" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="138" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="139" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="140" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="141" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="142" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="143" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="144" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="145" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="146" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="147" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="148" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="149" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="150" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="151" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="152" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="153" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="154" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="155" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="156" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="157" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="158" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="159" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="160" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="161" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="162" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="163" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="164" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="165" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="166" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="167" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="168" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="169" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="170" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="171" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="172" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="173" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="174" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="175" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="176" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="177" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="178" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="179" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="180" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="181" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="182" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="183" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="184" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="185" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="186" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="187" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="188" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="189" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="190" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="191" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="192" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="193" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="194" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="195" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="196" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="197" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="198" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="199" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="200" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="201" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="202" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="203" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="204" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="205" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="206" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="207" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="208" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="209" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="210" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="211" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="212" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="213" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="214" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="215" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="216" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="217" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="218" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="219" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="220" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="221" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="222" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="223" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="224" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="225" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="226" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="227" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="228" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="229" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="230" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="231" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:26" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="17" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="18" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="19" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="20" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="21" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="22" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="23" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="24" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="25" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="26" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="27" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="28" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="29" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="30" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="31" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="32" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="33" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="34" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="35" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="36" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="37" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="38" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="39" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="40" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="41" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="42" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="43" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="44" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="45" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="46" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="47" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="48" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="49" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="50" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="51" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="52" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="53" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="54" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="55" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="56" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="57" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="58" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="59" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="60" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="61" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="62" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="63" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="64" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="65" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="66" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="67" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="68" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="69" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="70" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="71" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="72" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="73" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="74" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="75" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="76" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="77" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="78" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="79" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="80" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="81" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="82" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="83" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="84" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="85" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="86" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="87" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="88" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="89" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="90" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="91" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="92" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="93" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="94" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="95" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="96" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="97" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="98" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="99" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="100" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="101" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="102" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="103" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="104" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="105" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="106" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="107" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="108" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="109" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="110" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="111" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="112" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="113" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="114" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="115" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="116" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="117" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="118" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="119" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="120" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="121" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="122" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="123" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="124" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="125" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="126" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="127" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="128" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="129" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="130" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="131" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="132" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="133" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="134" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="135" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="136" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="137" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="138" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="139" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="140" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="141" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="142" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="143" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="144" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="145" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="146" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="147" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="148" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="149" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="150" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="151" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="152" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="153" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="154" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="155" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="156" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="157" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="158" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="159" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="160" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="161" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="162" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="163" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="164" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="165" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="166" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="167" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="168" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="169" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="170" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="171" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="172" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="173" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="174" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="175" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="176" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="177" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="178" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="179" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="180" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="181" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="182" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="183" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="184" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="185" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="186" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="187" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="188" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="189" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="190" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="191" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="192" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="193" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="194" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="195" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="196" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="197" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="198" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="199" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="200" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="201" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="202" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="203" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="204" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="205" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="206" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="207" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="208" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="209" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="210" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="211" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="212" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="213" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="214" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="215" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="216" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="217" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="218" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="219" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="220" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="221" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="222" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="223" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="224" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="225" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="226" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="227" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="228" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="229" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="230" s="45" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="231" s="45" customFormat="1" ht="15.75" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1945,15 +1946,15 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z334"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="29.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
@@ -1962,7 +1963,7 @@
     <col min="7" max="7" width="48.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="45" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" s="45" customFormat="1" ht="30">
       <c r="A1" s="83" t="s">
         <v>0</v>
       </c>
@@ -1985,7 +1986,7 @@
       <c r="H1" s="58"/>
       <c r="I1" s="58"/>
     </row>
-    <row r="2" spans="1:26" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" s="45" customFormat="1" ht="15.75" customHeight="1">
       <c r="A2" s="87"/>
       <c r="B2" s="87"/>
       <c r="C2" s="63"/>
@@ -2013,7 +2014,7 @@
       <c r="Y2" s="67"/>
       <c r="Z2" s="67"/>
     </row>
-    <row r="3" spans="1:26" s="45" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" s="45" customFormat="1" ht="15">
       <c r="A3" s="79" t="s">
         <v>15</v>
       </c>
@@ -2051,7 +2052,7 @@
       <c r="Y3" s="67"/>
       <c r="Z3" s="67"/>
     </row>
-    <row r="4" spans="1:26" s="45" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" s="45" customFormat="1" ht="15">
       <c r="A4" s="79" t="s">
         <v>18</v>
       </c>
@@ -2089,7 +2090,7 @@
       <c r="Y4" s="67"/>
       <c r="Z4" s="67"/>
     </row>
-    <row r="5" spans="1:26" s="45" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" s="45" customFormat="1" ht="15">
       <c r="A5" s="79" t="s">
         <v>19</v>
       </c>
@@ -2127,7 +2128,7 @@
       <c r="Y5" s="67"/>
       <c r="Z5" s="67"/>
     </row>
-    <row r="6" spans="1:26" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" s="45" customFormat="1" ht="15.75" customHeight="1">
       <c r="A6" s="79"/>
       <c r="B6" s="87"/>
       <c r="C6" s="101"/>
@@ -2155,7 +2156,7 @@
       <c r="Y6" s="65"/>
       <c r="Z6" s="65"/>
     </row>
-    <row r="7" spans="1:26" s="45" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" s="45" customFormat="1" ht="15">
       <c r="A7" s="79" t="s">
         <v>22</v>
       </c>
@@ -2197,7 +2198,7 @@
       <c r="Y7" s="65"/>
       <c r="Z7" s="65"/>
     </row>
-    <row r="8" spans="1:26" s="45" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" s="45" customFormat="1" ht="15">
       <c r="A8" s="79" t="s">
         <v>22</v>
       </c>
@@ -2239,7 +2240,7 @@
       <c r="Y8" s="73"/>
       <c r="Z8" s="73"/>
     </row>
-    <row r="9" spans="1:26" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" s="45" customFormat="1" ht="15.75" customHeight="1">
       <c r="A9" s="79"/>
       <c r="B9" s="59"/>
       <c r="C9" s="101"/>
@@ -2267,7 +2268,7 @@
       <c r="Y9" s="67"/>
       <c r="Z9" s="67"/>
     </row>
-    <row r="10" spans="1:26" s="45" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" s="45" customFormat="1" ht="15">
       <c r="A10" s="89" t="s">
         <v>50</v>
       </c>
@@ -2305,7 +2306,7 @@
       <c r="Y10" s="73"/>
       <c r="Z10" s="73"/>
     </row>
-    <row r="11" spans="1:26" s="45" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" s="45" customFormat="1" ht="15">
       <c r="A11" s="89"/>
       <c r="B11" s="103"/>
       <c r="C11" s="101"/>
@@ -2333,7 +2334,7 @@
       <c r="Y11" s="65"/>
       <c r="Z11" s="65"/>
     </row>
-    <row r="12" spans="1:26" s="45" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" s="45" customFormat="1" ht="15">
       <c r="A12" s="91" t="s">
         <v>45</v>
       </c>
@@ -2375,7 +2376,7 @@
       <c r="Y12" s="73"/>
       <c r="Z12" s="73"/>
     </row>
-    <row r="13" spans="1:26" s="45" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" s="45" customFormat="1" ht="15">
       <c r="A13" s="87"/>
       <c r="B13" s="104"/>
       <c r="C13" s="101"/>
@@ -2403,7 +2404,7 @@
       <c r="Y13" s="73"/>
       <c r="Z13" s="73"/>
     </row>
-    <row r="14" spans="1:26" s="45" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" s="45" customFormat="1" ht="15">
       <c r="A14" s="87" t="s">
         <v>46</v>
       </c>
@@ -2443,7 +2444,7 @@
       <c r="Y14" s="73"/>
       <c r="Z14" s="73"/>
     </row>
-    <row r="15" spans="1:26" s="45" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" s="45" customFormat="1" ht="15">
       <c r="A15" s="87" t="s">
         <v>46</v>
       </c>
@@ -2483,7 +2484,7 @@
       <c r="Y15" s="73"/>
       <c r="Z15" s="73"/>
     </row>
-    <row r="16" spans="1:26" s="45" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" s="45" customFormat="1" ht="15">
       <c r="A16" s="87" t="s">
         <v>46</v>
       </c>
@@ -2525,7 +2526,7 @@
       <c r="Y16" s="73"/>
       <c r="Z16" s="73"/>
     </row>
-    <row r="17" spans="1:26" s="45" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" s="45" customFormat="1" ht="15">
       <c r="A17" s="87" t="s">
         <v>46</v>
       </c>
@@ -2565,7 +2566,7 @@
       <c r="Y17" s="73"/>
       <c r="Z17" s="73"/>
     </row>
-    <row r="18" spans="1:26" s="45" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" s="45" customFormat="1" ht="15">
       <c r="A18" s="87" t="s">
         <v>46</v>
       </c>
@@ -2605,7 +2606,7 @@
       <c r="Y18" s="65"/>
       <c r="Z18" s="65"/>
     </row>
-    <row r="19" spans="1:26" s="45" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" s="45" customFormat="1" ht="15">
       <c r="A19" s="87" t="s">
         <v>46</v>
       </c>
@@ -2645,7 +2646,7 @@
       <c r="Y19" s="65"/>
       <c r="Z19" s="65"/>
     </row>
-    <row r="20" spans="1:26" s="45" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" s="45" customFormat="1" ht="15">
       <c r="A20" s="87"/>
       <c r="B20" s="104"/>
       <c r="C20" s="101"/>
@@ -2673,7 +2674,7 @@
       <c r="Y20" s="65"/>
       <c r="Z20" s="65"/>
     </row>
-    <row r="21" spans="1:26" s="45" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" s="45" customFormat="1" ht="15">
       <c r="A21" s="87" t="s">
         <v>47</v>
       </c>
@@ -2713,7 +2714,7 @@
       <c r="Y21" s="65"/>
       <c r="Z21" s="65"/>
     </row>
-    <row r="22" spans="1:26" s="45" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26" s="45" customFormat="1" ht="15">
       <c r="A22" s="87" t="s">
         <v>47</v>
       </c>
@@ -2753,7 +2754,7 @@
       <c r="Y22" s="65"/>
       <c r="Z22" s="65"/>
     </row>
-    <row r="23" spans="1:26" s="45" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26" s="45" customFormat="1" ht="15">
       <c r="A23" s="87" t="s">
         <v>47</v>
       </c>
@@ -2793,7 +2794,7 @@
       <c r="Y23" s="65"/>
       <c r="Z23" s="65"/>
     </row>
-    <row r="24" spans="1:26" s="45" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:26" s="45" customFormat="1" ht="15">
       <c r="A24" s="87" t="s">
         <v>47</v>
       </c>
@@ -2832,7 +2833,7 @@
       <c r="Y24" s="65"/>
       <c r="Z24" s="65"/>
     </row>
-    <row r="25" spans="1:26" s="45" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:26" s="45" customFormat="1" ht="15">
       <c r="A25" s="87" t="s">
         <v>47</v>
       </c>
@@ -2871,7 +2872,7 @@
       <c r="Y25" s="65"/>
       <c r="Z25" s="65"/>
     </row>
-    <row r="26" spans="1:26" s="45" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:26" s="45" customFormat="1" ht="15">
       <c r="A26" s="87" t="s">
         <v>47</v>
       </c>
@@ -2909,7 +2910,7 @@
       <c r="Y26" s="73"/>
       <c r="Z26" s="73"/>
     </row>
-    <row r="27" spans="1:26" s="45" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:26" s="45" customFormat="1" ht="15">
       <c r="A27" s="93" t="s">
         <v>47</v>
       </c>
@@ -2949,7 +2950,7 @@
       <c r="Y27" s="73"/>
       <c r="Z27" s="73"/>
     </row>
-    <row r="28" spans="1:26" s="45" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:26" s="45" customFormat="1" ht="15">
       <c r="A28" s="93" t="s">
         <v>47</v>
       </c>
@@ -2989,7 +2990,7 @@
       <c r="Y28" s="73"/>
       <c r="Z28" s="73"/>
     </row>
-    <row r="29" spans="1:26" s="45" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:26" s="45" customFormat="1" ht="15">
       <c r="A29" s="87"/>
       <c r="B29" s="104"/>
       <c r="C29" s="101"/>
@@ -3017,7 +3018,7 @@
       <c r="Y29" s="73"/>
       <c r="Z29" s="73"/>
     </row>
-    <row r="30" spans="1:26" s="45" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:26" s="45" customFormat="1" ht="15">
       <c r="A30" s="87" t="s">
         <v>48</v>
       </c>
@@ -3057,7 +3058,7 @@
       <c r="Y30" s="73"/>
       <c r="Z30" s="73"/>
     </row>
-    <row r="31" spans="1:26" s="45" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:26" s="45" customFormat="1" ht="15">
       <c r="A31" s="87" t="s">
         <v>48</v>
       </c>
@@ -3097,7 +3098,7 @@
       <c r="Y31" s="73"/>
       <c r="Z31" s="73"/>
     </row>
-    <row r="32" spans="1:26" s="45" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:26" s="45" customFormat="1" ht="15">
       <c r="A32" s="87"/>
       <c r="B32" s="104"/>
       <c r="C32" s="101"/>
@@ -3125,7 +3126,7 @@
       <c r="Y32" s="73"/>
       <c r="Z32" s="73"/>
     </row>
-    <row r="33" spans="1:26" s="45" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:26" s="45" customFormat="1" ht="15">
       <c r="A33" s="96" t="s">
         <v>49</v>
       </c>
@@ -3165,7 +3166,7 @@
       <c r="Y33" s="73"/>
       <c r="Z33" s="73"/>
     </row>
-    <row r="34" spans="1:26" s="45" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:26" s="45" customFormat="1" ht="15">
       <c r="A34" s="96" t="s">
         <v>49</v>
       </c>
@@ -3205,7 +3206,7 @@
       <c r="Y34" s="73"/>
       <c r="Z34" s="73"/>
     </row>
-    <row r="57" spans="1:26" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:26" s="45" customFormat="1" ht="15.75" customHeight="1">
       <c r="A57" s="52"/>
       <c r="B57" s="52"/>
       <c r="C57" s="51"/>
@@ -3233,7 +3234,7 @@
       <c r="Y57" s="67"/>
       <c r="Z57" s="67"/>
     </row>
-    <row r="58" spans="1:26" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:26" s="45" customFormat="1" ht="15.75" customHeight="1">
       <c r="A58" s="52"/>
       <c r="B58" s="52"/>
       <c r="C58" s="51"/>
@@ -3261,7 +3262,7 @@
       <c r="Y58" s="67"/>
       <c r="Z58" s="67"/>
     </row>
-    <row r="59" spans="1:26" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:26" s="45" customFormat="1" ht="15.75" customHeight="1">
       <c r="A59" s="52"/>
       <c r="B59" s="52"/>
       <c r="C59" s="51"/>
@@ -3289,7 +3290,7 @@
       <c r="Y59" s="67"/>
       <c r="Z59" s="67"/>
     </row>
-    <row r="60" spans="1:26" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:26" s="45" customFormat="1" ht="15.75" customHeight="1">
       <c r="A60" s="52"/>
       <c r="B60" s="47"/>
       <c r="C60" s="51"/>
@@ -3317,7 +3318,7 @@
       <c r="Y60" s="67"/>
       <c r="Z60" s="67"/>
     </row>
-    <row r="61" spans="1:26" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:26" s="45" customFormat="1" ht="15.75" customHeight="1">
       <c r="A61" s="52"/>
       <c r="B61" s="47"/>
       <c r="C61" s="51"/>
@@ -3345,7 +3346,7 @@
       <c r="Y61" s="67"/>
       <c r="Z61" s="67"/>
     </row>
-    <row r="62" spans="1:26" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:26" s="45" customFormat="1" ht="15.75" customHeight="1">
       <c r="A62" s="52"/>
       <c r="B62" s="47"/>
       <c r="C62" s="51"/>
@@ -3373,7 +3374,7 @@
       <c r="Y62" s="67"/>
       <c r="Z62" s="67"/>
     </row>
-    <row r="63" spans="1:26" s="45" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:26" s="45" customFormat="1" ht="12.75">
       <c r="A63" s="52"/>
       <c r="B63" s="47"/>
       <c r="C63" s="51"/>
@@ -3401,7 +3402,7 @@
       <c r="Y63" s="67"/>
       <c r="Z63" s="67"/>
     </row>
-    <row r="64" spans="1:26" s="45" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:26" s="45" customFormat="1" ht="12.75">
       <c r="A64" s="52"/>
       <c r="B64" s="47"/>
       <c r="C64" s="51"/>
@@ -3429,7 +3430,7 @@
       <c r="Y64" s="67"/>
       <c r="Z64" s="67"/>
     </row>
-    <row r="65" spans="1:26" s="45" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:26" s="45" customFormat="1" ht="12.75">
       <c r="A65" s="52"/>
       <c r="B65" s="47"/>
       <c r="C65" s="51"/>
@@ -3457,7 +3458,7 @@
       <c r="Y65" s="67"/>
       <c r="Z65" s="67"/>
     </row>
-    <row r="66" spans="1:26" s="45" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:26" s="45" customFormat="1" ht="12.75">
       <c r="A66" s="52"/>
       <c r="B66" s="47"/>
       <c r="C66" s="51"/>
@@ -3485,7 +3486,7 @@
       <c r="Y66" s="67"/>
       <c r="Z66" s="67"/>
     </row>
-    <row r="67" spans="1:26" s="45" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:26" s="45" customFormat="1" ht="14.25">
       <c r="A67" s="70"/>
       <c r="B67" s="47"/>
       <c r="C67" s="51"/>
@@ -3513,7 +3514,7 @@
       <c r="Y67" s="67"/>
       <c r="Z67" s="67"/>
     </row>
-    <row r="68" spans="1:26" s="45" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:26" s="45" customFormat="1" ht="15">
       <c r="A68" s="52"/>
       <c r="B68" s="47"/>
       <c r="C68" s="51"/>
@@ -3541,7 +3542,7 @@
       <c r="Y68" s="67"/>
       <c r="Z68" s="67"/>
     </row>
-    <row r="69" spans="1:26" s="45" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:26" s="45" customFormat="1" ht="15">
       <c r="A69" s="52"/>
       <c r="B69" s="47"/>
       <c r="C69" s="51"/>
@@ -3569,7 +3570,7 @@
       <c r="Y69" s="67"/>
       <c r="Z69" s="67"/>
     </row>
-    <row r="70" spans="1:26" s="45" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:26" s="45" customFormat="1" ht="12.75">
       <c r="A70" s="52"/>
       <c r="B70" s="47"/>
       <c r="C70" s="51"/>
@@ -3597,7 +3598,7 @@
       <c r="Y70" s="67"/>
       <c r="Z70" s="67"/>
     </row>
-    <row r="71" spans="1:26" s="45" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:26" s="45" customFormat="1" ht="12.75">
       <c r="A71" s="52"/>
       <c r="B71" s="47"/>
       <c r="C71" s="51"/>
@@ -3625,7 +3626,7 @@
       <c r="Y71" s="67"/>
       <c r="Z71" s="67"/>
     </row>
-    <row r="72" spans="1:26" s="45" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:26" s="45" customFormat="1" ht="12.75">
       <c r="A72" s="52"/>
       <c r="B72" s="47"/>
       <c r="C72" s="51"/>
@@ -3653,7 +3654,7 @@
       <c r="Y72" s="67"/>
       <c r="Z72" s="67"/>
     </row>
-    <row r="73" spans="1:26" s="45" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:26" s="45" customFormat="1" ht="12.75">
       <c r="A73" s="52"/>
       <c r="B73" s="47"/>
       <c r="C73" s="51"/>
@@ -3681,7 +3682,7 @@
       <c r="Y73" s="67"/>
       <c r="Z73" s="67"/>
     </row>
-    <row r="74" spans="1:26" s="45" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:26" s="45" customFormat="1" ht="14.25">
       <c r="A74" s="70"/>
       <c r="B74" s="47"/>
       <c r="C74" s="51"/>
@@ -3709,7 +3710,7 @@
       <c r="Y74" s="67"/>
       <c r="Z74" s="67"/>
     </row>
-    <row r="75" spans="1:26" s="45" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:26" s="45" customFormat="1" ht="15">
       <c r="A75" s="65"/>
       <c r="B75" s="52"/>
       <c r="C75" s="51"/>
@@ -3737,7 +3738,7 @@
       <c r="Y75" s="67"/>
       <c r="Z75" s="67"/>
     </row>
-    <row r="76" spans="1:26" s="45" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:26" s="45" customFormat="1" ht="12.75">
       <c r="A76" s="65"/>
       <c r="B76" s="65"/>
       <c r="C76" s="48"/>
@@ -3765,7 +3766,7 @@
       <c r="Y76" s="67"/>
       <c r="Z76" s="67"/>
     </row>
-    <row r="77" spans="1:26" s="45" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:26" s="45" customFormat="1" ht="12.75">
       <c r="A77" s="65"/>
       <c r="B77" s="73"/>
       <c r="C77" s="73"/>
@@ -3793,7 +3794,7 @@
       <c r="Y77" s="67"/>
       <c r="Z77" s="67"/>
     </row>
-    <row r="78" spans="1:26" s="45" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:26" s="45" customFormat="1" ht="12.75">
       <c r="A78" s="65"/>
       <c r="B78" s="73"/>
       <c r="C78" s="73"/>
@@ -3821,7 +3822,7 @@
       <c r="Y78" s="67"/>
       <c r="Z78" s="67"/>
     </row>
-    <row r="79" spans="1:26" s="45" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:26" s="45" customFormat="1" ht="12.75">
       <c r="A79" s="65"/>
       <c r="B79" s="65"/>
       <c r="C79" s="65"/>
@@ -3849,7 +3850,7 @@
       <c r="Y79" s="67"/>
       <c r="Z79" s="67"/>
     </row>
-    <row r="80" spans="1:26" s="45" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:26" s="45" customFormat="1" ht="12.75">
       <c r="A80" s="65"/>
       <c r="B80" s="65"/>
       <c r="C80" s="65"/>
@@ -3877,7 +3878,7 @@
       <c r="Y80" s="67"/>
       <c r="Z80" s="67"/>
     </row>
-    <row r="81" spans="1:26" s="45" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:26" s="45" customFormat="1" ht="12.75">
       <c r="A81" s="65"/>
       <c r="B81" s="65"/>
       <c r="C81" s="65"/>
@@ -3905,7 +3906,7 @@
       <c r="Y81" s="67"/>
       <c r="Z81" s="67"/>
     </row>
-    <row r="82" spans="1:26" s="45" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:26" s="45" customFormat="1" ht="12.75">
       <c r="A82" s="65"/>
       <c r="B82" s="65"/>
       <c r="C82" s="65"/>
@@ -3933,7 +3934,7 @@
       <c r="Y82" s="67"/>
       <c r="Z82" s="67"/>
     </row>
-    <row r="83" spans="1:26" s="45" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:26" s="45" customFormat="1" ht="12.75">
       <c r="A83" s="65"/>
       <c r="B83" s="65"/>
       <c r="C83" s="65"/>
@@ -3961,7 +3962,7 @@
       <c r="Y83" s="67"/>
       <c r="Z83" s="67"/>
     </row>
-    <row r="84" spans="1:26" s="45" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:26" s="45" customFormat="1" ht="12.75">
       <c r="A84" s="65"/>
       <c r="B84" s="73"/>
       <c r="C84" s="73"/>
@@ -3989,7 +3990,7 @@
       <c r="Y84" s="67"/>
       <c r="Z84" s="67"/>
     </row>
-    <row r="85" spans="1:26" s="45" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:26" s="45" customFormat="1" ht="12.75">
       <c r="A85" s="65"/>
       <c r="B85" s="73"/>
       <c r="C85" s="73"/>
@@ -4017,7 +4018,7 @@
       <c r="Y85" s="67"/>
       <c r="Z85" s="67"/>
     </row>
-    <row r="86" spans="1:26" s="45" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:26" s="45" customFormat="1" ht="12.75">
       <c r="A86" s="65"/>
       <c r="B86" s="73"/>
       <c r="C86" s="73"/>
@@ -4045,7 +4046,7 @@
       <c r="Y86" s="67"/>
       <c r="Z86" s="67"/>
     </row>
-    <row r="87" spans="1:26" s="45" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:26" s="45" customFormat="1" ht="12.75">
       <c r="A87" s="65"/>
       <c r="B87" s="73"/>
       <c r="C87" s="73"/>
@@ -4073,7 +4074,7 @@
       <c r="Y87" s="67"/>
       <c r="Z87" s="67"/>
     </row>
-    <row r="88" spans="1:26" s="45" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:26" s="45" customFormat="1" ht="12.75">
       <c r="A88" s="65"/>
       <c r="B88" s="73"/>
       <c r="C88" s="73"/>
@@ -4101,7 +4102,7 @@
       <c r="Y88" s="67"/>
       <c r="Z88" s="67"/>
     </row>
-    <row r="89" spans="1:26" s="45" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:26" s="45" customFormat="1" ht="15">
       <c r="A89" s="65"/>
       <c r="B89" s="67"/>
       <c r="C89" s="68"/>
@@ -4129,7 +4130,7 @@
       <c r="Y89" s="67"/>
       <c r="Z89" s="67"/>
     </row>
-    <row r="90" spans="1:26" s="45" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:26" s="45" customFormat="1" ht="15">
       <c r="A90" s="52"/>
       <c r="B90" s="52"/>
       <c r="C90" s="51"/>
@@ -4157,7 +4158,7 @@
       <c r="Y90" s="67"/>
       <c r="Z90" s="67"/>
     </row>
-    <row r="91" spans="1:26" s="45" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:26" s="45" customFormat="1" ht="15">
       <c r="A91" s="52"/>
       <c r="B91" s="52"/>
       <c r="C91" s="51"/>
@@ -4185,7 +4186,7 @@
       <c r="Y91" s="67"/>
       <c r="Z91" s="67"/>
     </row>
-    <row r="92" spans="1:26" s="45" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:26" s="45" customFormat="1" ht="15">
       <c r="A92" s="52"/>
       <c r="B92" s="67"/>
       <c r="C92" s="68"/>
@@ -4213,7 +4214,7 @@
       <c r="Y92" s="67"/>
       <c r="Z92" s="67"/>
     </row>
-    <row r="93" spans="1:26" s="45" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:26" s="45" customFormat="1" ht="15">
       <c r="A93" s="52"/>
       <c r="B93" s="52"/>
       <c r="C93" s="51"/>
@@ -4241,7 +4242,7 @@
       <c r="Y93" s="67"/>
       <c r="Z93" s="67"/>
     </row>
-    <row r="94" spans="1:26" s="45" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:26" s="45" customFormat="1" ht="15">
       <c r="A94" s="52"/>
       <c r="B94" s="52"/>
       <c r="C94" s="51"/>
@@ -4269,7 +4270,7 @@
       <c r="Y94" s="67"/>
       <c r="Z94" s="67"/>
     </row>
-    <row r="95" spans="1:26" s="45" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:26" s="45" customFormat="1" ht="15">
       <c r="A95" s="52"/>
       <c r="B95" s="67"/>
       <c r="C95" s="68"/>
@@ -4297,7 +4298,7 @@
       <c r="Y95" s="67"/>
       <c r="Z95" s="67"/>
     </row>
-    <row r="96" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:26" ht="15">
       <c r="A96" s="2"/>
       <c r="B96" s="2"/>
       <c r="C96" s="3"/>
@@ -4325,7 +4326,7 @@
       <c r="Y96" s="6"/>
       <c r="Z96" s="6"/>
     </row>
-    <row r="97" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:26" ht="15">
       <c r="A97" s="2"/>
       <c r="B97" s="2"/>
       <c r="C97" s="3"/>
@@ -4353,7 +4354,7 @@
       <c r="Y97" s="6"/>
       <c r="Z97" s="6"/>
     </row>
-    <row r="98" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:26" ht="14.25">
       <c r="A98" s="11"/>
       <c r="B98" s="10"/>
       <c r="C98" s="3"/>
@@ -4381,7 +4382,7 @@
       <c r="Y98" s="6"/>
       <c r="Z98" s="6"/>
     </row>
-    <row r="99" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:26" ht="15">
       <c r="A99" s="2"/>
       <c r="B99" s="2"/>
       <c r="C99" s="8"/>
@@ -4409,7 +4410,7 @@
       <c r="Y99" s="6"/>
       <c r="Z99" s="6"/>
     </row>
-    <row r="100" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:26" ht="15">
       <c r="A100" s="2"/>
       <c r="B100" s="2"/>
       <c r="C100" s="8"/>
@@ -4437,7 +4438,7 @@
       <c r="Y100" s="6"/>
       <c r="Z100" s="6"/>
     </row>
-    <row r="101" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:26" ht="14.25">
       <c r="A101" s="11"/>
       <c r="B101" s="10"/>
       <c r="C101" s="3"/>
@@ -4465,7 +4466,7 @@
       <c r="Y101" s="6"/>
       <c r="Z101" s="6"/>
     </row>
-    <row r="102" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:26" ht="15">
       <c r="A102" s="2"/>
       <c r="B102" s="10"/>
       <c r="C102" s="8"/>
@@ -4493,7 +4494,7 @@
       <c r="Y102" s="6"/>
       <c r="Z102" s="6"/>
     </row>
-    <row r="103" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:26" ht="15">
       <c r="A103" s="2"/>
       <c r="B103" s="10"/>
       <c r="C103" s="8"/>
@@ -4521,7 +4522,7 @@
       <c r="Y103" s="6"/>
       <c r="Z103" s="6"/>
     </row>
-    <row r="104" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:26" ht="14.25">
       <c r="A104" s="11"/>
       <c r="B104" s="10"/>
       <c r="C104" s="3"/>
@@ -4549,7 +4550,7 @@
       <c r="Y104" s="6"/>
       <c r="Z104" s="6"/>
     </row>
-    <row r="105" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:26" ht="15">
       <c r="A105" s="2"/>
       <c r="B105" s="10"/>
       <c r="C105" s="8"/>
@@ -4577,7 +4578,7 @@
       <c r="Y105" s="6"/>
       <c r="Z105" s="6"/>
     </row>
-    <row r="106" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:26" ht="15">
       <c r="A106" s="2"/>
       <c r="B106" s="10"/>
       <c r="C106" s="8"/>
@@ -4605,7 +4606,7 @@
       <c r="Y106" s="6"/>
       <c r="Z106" s="6"/>
     </row>
-    <row r="107" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:26" ht="14.25">
       <c r="A107" s="11"/>
       <c r="B107" s="10"/>
       <c r="C107" s="3"/>
@@ -4633,7 +4634,7 @@
       <c r="Y107" s="6"/>
       <c r="Z107" s="6"/>
     </row>
-    <row r="108" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:26" ht="12.75">
       <c r="A108" s="11"/>
       <c r="B108" s="13"/>
       <c r="C108" s="3"/>
@@ -4661,7 +4662,7 @@
       <c r="Y108" s="6"/>
       <c r="Z108" s="6"/>
     </row>
-    <row r="109" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:26" ht="12.75">
       <c r="A109" s="11"/>
       <c r="B109" s="13"/>
       <c r="C109" s="3"/>
@@ -4689,7 +4690,7 @@
       <c r="Y109" s="6"/>
       <c r="Z109" s="6"/>
     </row>
-    <row r="110" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:26" ht="12.75">
       <c r="A110" s="11"/>
       <c r="B110" s="13"/>
       <c r="C110" s="3"/>
@@ -4717,7 +4718,7 @@
       <c r="Y110" s="6"/>
       <c r="Z110" s="6"/>
     </row>
-    <row r="111" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:26" ht="12.75">
       <c r="A111" s="11"/>
       <c r="B111" s="13"/>
       <c r="C111" s="3"/>
@@ -4745,7 +4746,7 @@
       <c r="Y111" s="6"/>
       <c r="Z111" s="6"/>
     </row>
-    <row r="112" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:26" ht="12.75">
       <c r="A112" s="11"/>
       <c r="B112" s="13"/>
       <c r="C112" s="3"/>
@@ -4773,7 +4774,7 @@
       <c r="Y112" s="6"/>
       <c r="Z112" s="6"/>
     </row>
-    <row r="113" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:26" ht="14.25">
       <c r="A113" s="11"/>
       <c r="B113" s="10"/>
       <c r="C113" s="3"/>
@@ -4801,7 +4802,7 @@
       <c r="Y113" s="6"/>
       <c r="Z113" s="6"/>
     </row>
-    <row r="114" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:26" ht="14.25">
       <c r="A114" s="2"/>
       <c r="B114" s="2"/>
       <c r="C114" s="8"/>
@@ -4829,7 +4830,7 @@
       <c r="Y114" s="6"/>
       <c r="Z114" s="6"/>
     </row>
-    <row r="115" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:26" ht="14.25">
       <c r="A115" s="2"/>
       <c r="B115" s="2"/>
       <c r="C115" s="8"/>
@@ -4857,7 +4858,7 @@
       <c r="Y115" s="6"/>
       <c r="Z115" s="6"/>
     </row>
-    <row r="116" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:26" ht="14.25">
       <c r="A116" s="2"/>
       <c r="B116" s="2"/>
       <c r="C116" s="8"/>
@@ -4885,7 +4886,7 @@
       <c r="Y116" s="6"/>
       <c r="Z116" s="6"/>
     </row>
-    <row r="117" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:26" ht="14.25">
       <c r="A117" s="2"/>
       <c r="B117" s="2"/>
       <c r="C117" s="8"/>
@@ -4913,7 +4914,7 @@
       <c r="Y117" s="6"/>
       <c r="Z117" s="6"/>
     </row>
-    <row r="118" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:26" ht="14.25">
       <c r="A118" s="2"/>
       <c r="B118" s="2"/>
       <c r="C118" s="8"/>
@@ -4941,7 +4942,7 @@
       <c r="Y118" s="6"/>
       <c r="Z118" s="6"/>
     </row>
-    <row r="119" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:26" ht="14.25">
       <c r="A119" s="11"/>
       <c r="B119" s="10"/>
       <c r="C119" s="3"/>
@@ -4969,7 +4970,7 @@
       <c r="Y119" s="6"/>
       <c r="Z119" s="6"/>
     </row>
-    <row r="120" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:26" ht="14.25">
       <c r="A120" s="11"/>
       <c r="B120" s="10"/>
       <c r="C120" s="3"/>
@@ -4997,7 +4998,7 @@
       <c r="Y120" s="6"/>
       <c r="Z120" s="6"/>
     </row>
-    <row r="121" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:26" ht="14.25">
       <c r="A121" s="11"/>
       <c r="B121" s="13"/>
       <c r="C121" s="3"/>
@@ -5025,7 +5026,7 @@
       <c r="Y121" s="6"/>
       <c r="Z121" s="6"/>
     </row>
-    <row r="122" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:26" ht="14.25">
       <c r="A122" s="11"/>
       <c r="B122" s="13"/>
       <c r="C122" s="3"/>
@@ -5053,7 +5054,7 @@
       <c r="Y122" s="6"/>
       <c r="Z122" s="6"/>
     </row>
-    <row r="123" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:26" ht="14.25">
       <c r="A123" s="11"/>
       <c r="B123" s="10"/>
       <c r="C123" s="3"/>
@@ -5081,7 +5082,7 @@
       <c r="Y123" s="6"/>
       <c r="Z123" s="6"/>
     </row>
-    <row r="124" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:26" ht="14.25">
       <c r="A124" s="2"/>
       <c r="B124" s="10"/>
       <c r="C124" s="8"/>
@@ -5109,7 +5110,7 @@
       <c r="Y124" s="6"/>
       <c r="Z124" s="6"/>
     </row>
-    <row r="125" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:26" ht="14.25">
       <c r="A125" s="2"/>
       <c r="B125" s="10"/>
       <c r="C125" s="8"/>
@@ -5137,7 +5138,7 @@
       <c r="Y125" s="6"/>
       <c r="Z125" s="6"/>
     </row>
-    <row r="126" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:26" ht="14.25">
       <c r="A126" s="2"/>
       <c r="B126" s="10"/>
       <c r="C126" s="8"/>
@@ -5165,7 +5166,7 @@
       <c r="Y126" s="6"/>
       <c r="Z126" s="6"/>
     </row>
-    <row r="127" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:26" ht="14.25">
       <c r="A127" s="11"/>
       <c r="B127" s="10"/>
       <c r="C127" s="3"/>
@@ -5193,7 +5194,7 @@
       <c r="Y127" s="6"/>
       <c r="Z127" s="6"/>
     </row>
-    <row r="128" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:26" ht="12.75">
       <c r="A128" s="7"/>
       <c r="B128" s="2"/>
       <c r="C128" s="3"/>
@@ -5221,7 +5222,7 @@
       <c r="Y128" s="6"/>
       <c r="Z128" s="6"/>
     </row>
-    <row r="129" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:26" ht="12.75">
       <c r="A129" s="2"/>
       <c r="B129" s="2"/>
       <c r="C129" s="3"/>
@@ -5249,7 +5250,7 @@
       <c r="Y129" s="6"/>
       <c r="Z129" s="6"/>
     </row>
-    <row r="130" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:26" ht="12.75">
       <c r="A130" s="2"/>
       <c r="B130" s="2"/>
       <c r="C130" s="3"/>
@@ -5277,7 +5278,7 @@
       <c r="Y130" s="6"/>
       <c r="Z130" s="6"/>
     </row>
-    <row r="131" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:26" ht="12.75">
       <c r="A131" s="2"/>
       <c r="B131" s="2"/>
       <c r="C131" s="3"/>
@@ -5305,7 +5306,7 @@
       <c r="Y131" s="6"/>
       <c r="Z131" s="6"/>
     </row>
-    <row r="132" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:26" ht="12.75">
       <c r="A132" s="2"/>
       <c r="B132" s="2"/>
       <c r="C132" s="3"/>
@@ -5333,7 +5334,7 @@
       <c r="Y132" s="6"/>
       <c r="Z132" s="6"/>
     </row>
-    <row r="133" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:26" ht="12.75">
       <c r="A133" s="2"/>
       <c r="B133" s="2"/>
       <c r="C133" s="3"/>
@@ -5361,7 +5362,7 @@
       <c r="Y133" s="6"/>
       <c r="Z133" s="6"/>
     </row>
-    <row r="134" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:26" ht="12.75">
       <c r="A134" s="2"/>
       <c r="B134" s="2"/>
       <c r="C134" s="3"/>
@@ -5389,7 +5390,7 @@
       <c r="Y134" s="6"/>
       <c r="Z134" s="6"/>
     </row>
-    <row r="135" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:26" ht="12.75">
       <c r="A135" s="2"/>
       <c r="B135" s="2"/>
       <c r="C135" s="3"/>
@@ -5417,7 +5418,7 @@
       <c r="Y135" s="6"/>
       <c r="Z135" s="6"/>
     </row>
-    <row r="136" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:26" ht="12.75">
       <c r="A136" s="2"/>
       <c r="B136" s="2"/>
       <c r="C136" s="3"/>
@@ -5445,7 +5446,7 @@
       <c r="Y136" s="6"/>
       <c r="Z136" s="6"/>
     </row>
-    <row r="137" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:26" ht="12.75">
       <c r="A137" s="2"/>
       <c r="B137" s="2"/>
       <c r="C137" s="3"/>
@@ -5473,7 +5474,7 @@
       <c r="Y137" s="6"/>
       <c r="Z137" s="6"/>
     </row>
-    <row r="138" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:26" ht="12.75">
       <c r="A138" s="2"/>
       <c r="B138" s="2"/>
       <c r="C138" s="3"/>
@@ -5501,7 +5502,7 @@
       <c r="Y138" s="6"/>
       <c r="Z138" s="6"/>
     </row>
-    <row r="139" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:26" ht="12.75">
       <c r="A139" s="2"/>
       <c r="B139" s="2"/>
       <c r="C139" s="3"/>
@@ -5529,7 +5530,7 @@
       <c r="Y139" s="6"/>
       <c r="Z139" s="6"/>
     </row>
-    <row r="140" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:26" ht="12.75">
       <c r="A140" s="2"/>
       <c r="B140" s="2"/>
       <c r="C140" s="3"/>
@@ -5557,7 +5558,7 @@
       <c r="Y140" s="6"/>
       <c r="Z140" s="6"/>
     </row>
-    <row r="141" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:26" ht="12.75">
       <c r="A141" s="2"/>
       <c r="B141" s="2"/>
       <c r="C141" s="3"/>
@@ -5585,7 +5586,7 @@
       <c r="Y141" s="6"/>
       <c r="Z141" s="6"/>
     </row>
-    <row r="142" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:26" ht="12.75">
       <c r="A142" s="2"/>
       <c r="B142" s="2"/>
       <c r="C142" s="3"/>
@@ -5613,7 +5614,7 @@
       <c r="Y142" s="6"/>
       <c r="Z142" s="6"/>
     </row>
-    <row r="143" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:26" ht="12.75">
       <c r="A143" s="2"/>
       <c r="B143" s="2"/>
       <c r="C143" s="3"/>
@@ -5641,7 +5642,7 @@
       <c r="Y143" s="6"/>
       <c r="Z143" s="6"/>
     </row>
-    <row r="144" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:26" ht="12.75">
       <c r="A144" s="2"/>
       <c r="B144" s="2"/>
       <c r="C144" s="3"/>
@@ -5669,7 +5670,7 @@
       <c r="Y144" s="6"/>
       <c r="Z144" s="6"/>
     </row>
-    <row r="145" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:26" ht="12.75">
       <c r="A145" s="2"/>
       <c r="B145" s="2"/>
       <c r="C145" s="3"/>
@@ -5697,7 +5698,7 @@
       <c r="Y145" s="6"/>
       <c r="Z145" s="6"/>
     </row>
-    <row r="146" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:26" ht="12.75">
       <c r="A146" s="2"/>
       <c r="B146" s="2"/>
       <c r="C146" s="3"/>
@@ -5725,7 +5726,7 @@
       <c r="Y146" s="6"/>
       <c r="Z146" s="6"/>
     </row>
-    <row r="147" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:26" ht="12.75">
       <c r="A147" s="2"/>
       <c r="B147" s="2"/>
       <c r="C147" s="3"/>
@@ -5753,7 +5754,7 @@
       <c r="Y147" s="6"/>
       <c r="Z147" s="6"/>
     </row>
-    <row r="148" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:26" ht="12.75">
       <c r="A148" s="2"/>
       <c r="B148" s="2"/>
       <c r="C148" s="3"/>
@@ -5781,7 +5782,7 @@
       <c r="Y148" s="6"/>
       <c r="Z148" s="6"/>
     </row>
-    <row r="149" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:26" ht="12.75">
       <c r="A149" s="2"/>
       <c r="B149" s="2"/>
       <c r="C149" s="3"/>
@@ -5809,7 +5810,7 @@
       <c r="Y149" s="6"/>
       <c r="Z149" s="6"/>
     </row>
-    <row r="150" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:26" ht="12.75">
       <c r="A150" s="2"/>
       <c r="B150" s="2"/>
       <c r="C150" s="3"/>
@@ -5837,7 +5838,7 @@
       <c r="Y150" s="6"/>
       <c r="Z150" s="6"/>
     </row>
-    <row r="151" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:26" ht="12.75">
       <c r="A151" s="2"/>
       <c r="B151" s="2"/>
       <c r="C151" s="3"/>
@@ -5865,7 +5866,7 @@
       <c r="Y151" s="6"/>
       <c r="Z151" s="6"/>
     </row>
-    <row r="152" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:26" ht="12.75">
       <c r="A152" s="2"/>
       <c r="B152" s="2"/>
       <c r="C152" s="3"/>
@@ -5893,7 +5894,7 @@
       <c r="Y152" s="6"/>
       <c r="Z152" s="6"/>
     </row>
-    <row r="153" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:26" ht="12.75">
       <c r="A153" s="2"/>
       <c r="B153" s="2"/>
       <c r="C153" s="3"/>
@@ -5921,7 +5922,7 @@
       <c r="Y153" s="6"/>
       <c r="Z153" s="6"/>
     </row>
-    <row r="154" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:26" ht="12.75">
       <c r="A154" s="2"/>
       <c r="B154" s="2"/>
       <c r="C154" s="3"/>
@@ -5949,7 +5950,7 @@
       <c r="Y154" s="6"/>
       <c r="Z154" s="6"/>
     </row>
-    <row r="155" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:26" ht="12.75">
       <c r="A155" s="4"/>
       <c r="B155" s="4"/>
       <c r="C155" s="22"/>
@@ -5977,7 +5978,7 @@
       <c r="Y155" s="6"/>
       <c r="Z155" s="6"/>
     </row>
-    <row r="156" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:26" ht="15">
       <c r="A156" s="7"/>
       <c r="B156" s="2"/>
       <c r="C156" s="3"/>
@@ -6005,7 +6006,7 @@
       <c r="Y156" s="6"/>
       <c r="Z156" s="6"/>
     </row>
-    <row r="157" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:26" ht="15">
       <c r="A157" s="7"/>
       <c r="B157" s="10"/>
       <c r="C157" s="3"/>
@@ -6033,7 +6034,7 @@
       <c r="Y157" s="6"/>
       <c r="Z157" s="6"/>
     </row>
-    <row r="158" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:26" ht="12.75">
       <c r="A158" s="4"/>
       <c r="B158" s="4"/>
       <c r="C158" s="22"/>
@@ -6061,7 +6062,7 @@
       <c r="Y158" s="6"/>
       <c r="Z158" s="6"/>
     </row>
-    <row r="159" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:26" ht="15">
       <c r="A159" s="2"/>
       <c r="B159" s="2"/>
       <c r="C159" s="3"/>
@@ -6089,7 +6090,7 @@
       <c r="Y159" s="6"/>
       <c r="Z159" s="6"/>
     </row>
-    <row r="160" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:26" ht="15">
       <c r="A160" s="2"/>
       <c r="B160" s="2"/>
       <c r="C160" s="3"/>
@@ -6117,7 +6118,7 @@
       <c r="Y160" s="6"/>
       <c r="Z160" s="6"/>
     </row>
-    <row r="161" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:26" ht="12.75">
       <c r="A161" s="2"/>
       <c r="B161" s="4"/>
       <c r="C161" s="22"/>
@@ -6145,7 +6146,7 @@
       <c r="Y161" s="6"/>
       <c r="Z161" s="6"/>
     </row>
-    <row r="162" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:26" ht="15">
       <c r="A162" s="2"/>
       <c r="B162" s="7"/>
       <c r="C162" s="3"/>
@@ -6173,7 +6174,7 @@
       <c r="Y162" s="6"/>
       <c r="Z162" s="6"/>
     </row>
-    <row r="163" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:26" ht="15">
       <c r="A163" s="2"/>
       <c r="B163" s="7"/>
       <c r="C163" s="3"/>
@@ -6201,7 +6202,7 @@
       <c r="Y163" s="6"/>
       <c r="Z163" s="6"/>
     </row>
-    <row r="164" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:26" ht="12.75">
       <c r="A164" s="4"/>
       <c r="B164" s="4"/>
       <c r="C164" s="22"/>
@@ -6229,7 +6230,7 @@
       <c r="Y164" s="6"/>
       <c r="Z164" s="6"/>
     </row>
-    <row r="165" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:26" ht="15">
       <c r="A165" s="7"/>
       <c r="B165" s="2"/>
       <c r="C165" s="3"/>
@@ -6257,7 +6258,7 @@
       <c r="Y165" s="6"/>
       <c r="Z165" s="6"/>
     </row>
-    <row r="166" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:26" ht="15">
       <c r="A166" s="7"/>
       <c r="B166" s="2"/>
       <c r="C166" s="3"/>
@@ -6285,7 +6286,7 @@
       <c r="Y166" s="6"/>
       <c r="Z166" s="6"/>
     </row>
-    <row r="167" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:26" ht="12.75">
       <c r="A167" s="4"/>
       <c r="B167" s="23"/>
       <c r="C167" s="24"/>
@@ -6313,7 +6314,7 @@
       <c r="Y167" s="6"/>
       <c r="Z167" s="6"/>
     </row>
-    <row r="168" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:26" ht="15">
       <c r="A168" s="2"/>
       <c r="B168" s="31"/>
       <c r="C168" s="3"/>
@@ -6341,7 +6342,7 @@
       <c r="Y168" s="6"/>
       <c r="Z168" s="6"/>
     </row>
-    <row r="169" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:26" ht="15">
       <c r="A169" s="2"/>
       <c r="B169" s="31"/>
       <c r="C169" s="3"/>
@@ -6369,7 +6370,7 @@
       <c r="Y169" s="6"/>
       <c r="Z169" s="6"/>
     </row>
-    <row r="170" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:26" ht="12.75">
       <c r="A170" s="2"/>
       <c r="B170" s="23"/>
       <c r="C170" s="24"/>
@@ -6397,7 +6398,7 @@
       <c r="Y170" s="6"/>
       <c r="Z170" s="6"/>
     </row>
-    <row r="171" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:26" ht="15">
       <c r="A171" s="2"/>
       <c r="B171" s="31"/>
       <c r="C171" s="3"/>
@@ -6425,7 +6426,7 @@
       <c r="Y171" s="6"/>
       <c r="Z171" s="6"/>
     </row>
-    <row r="172" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:26" ht="15">
       <c r="A172" s="2"/>
       <c r="B172" s="31"/>
       <c r="C172" s="3"/>
@@ -6453,7 +6454,7 @@
       <c r="Y172" s="6"/>
       <c r="Z172" s="6"/>
     </row>
-    <row r="173" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:26" ht="12.75">
       <c r="A173" s="2"/>
       <c r="B173" s="23"/>
       <c r="C173" s="24"/>
@@ -6481,7 +6482,7 @@
       <c r="Y173" s="6"/>
       <c r="Z173" s="6"/>
     </row>
-    <row r="174" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:26" ht="15">
       <c r="A174" s="2"/>
       <c r="B174" s="2"/>
       <c r="C174" s="3"/>
@@ -6509,7 +6510,7 @@
       <c r="Y174" s="6"/>
       <c r="Z174" s="6"/>
     </row>
-    <row r="175" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:26" ht="15">
       <c r="A175" s="2"/>
       <c r="B175" s="2"/>
       <c r="C175" s="3"/>
@@ -6537,7 +6538,7 @@
       <c r="Y175" s="6"/>
       <c r="Z175" s="6"/>
     </row>
-    <row r="176" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:26" ht="12.75">
       <c r="A176" s="4"/>
       <c r="B176" s="23"/>
       <c r="C176" s="24"/>
@@ -6565,7 +6566,7 @@
       <c r="Y176" s="6"/>
       <c r="Z176" s="6"/>
     </row>
-    <row r="177" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:26" ht="15">
       <c r="A177" s="7"/>
       <c r="B177" s="10"/>
       <c r="C177" s="3"/>
@@ -6593,7 +6594,7 @@
       <c r="Y177" s="6"/>
       <c r="Z177" s="6"/>
     </row>
-    <row r="178" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:26" ht="15">
       <c r="A178" s="7"/>
       <c r="B178" s="10"/>
       <c r="C178" s="3"/>
@@ -6621,7 +6622,7 @@
       <c r="Y178" s="6"/>
       <c r="Z178" s="6"/>
     </row>
-    <row r="179" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:26" ht="12.75">
       <c r="A179" s="4"/>
       <c r="B179" s="23"/>
       <c r="C179" s="24"/>
@@ -6649,7 +6650,7 @@
       <c r="Y179" s="6"/>
       <c r="Z179" s="6"/>
     </row>
-    <row r="180" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:26" ht="15">
       <c r="A180" s="2"/>
       <c r="B180" s="2"/>
       <c r="C180" s="3"/>
@@ -6677,7 +6678,7 @@
       <c r="Y180" s="6"/>
       <c r="Z180" s="6"/>
     </row>
-    <row r="181" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:26" ht="15">
       <c r="A181" s="2"/>
       <c r="B181" s="2"/>
       <c r="C181" s="3"/>
@@ -6705,7 +6706,7 @@
       <c r="Y181" s="6"/>
       <c r="Z181" s="6"/>
     </row>
-    <row r="182" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:26" ht="12.75">
       <c r="A182" s="6"/>
       <c r="B182" s="6"/>
       <c r="C182" s="21"/>
@@ -6733,7 +6734,7 @@
       <c r="Y182" s="6"/>
       <c r="Z182" s="6"/>
     </row>
-    <row r="183" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:26" ht="12.75">
       <c r="A183" s="2"/>
       <c r="B183" s="6"/>
       <c r="C183" s="21"/>
@@ -6761,7 +6762,7 @@
       <c r="Y183" s="6"/>
       <c r="Z183" s="6"/>
     </row>
-    <row r="184" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:26" ht="12.75">
       <c r="A184" s="6"/>
       <c r="B184" s="6"/>
       <c r="C184" s="21"/>
@@ -6789,7 +6790,7 @@
       <c r="Y184" s="6"/>
       <c r="Z184" s="6"/>
     </row>
-    <row r="185" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:26" ht="12.75">
       <c r="A185" s="6"/>
       <c r="B185" s="6"/>
       <c r="C185" s="21"/>
@@ -6817,7 +6818,7 @@
       <c r="Y185" s="6"/>
       <c r="Z185" s="6"/>
     </row>
-    <row r="186" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:26" ht="12.75">
       <c r="A186" s="11"/>
       <c r="B186" s="2"/>
       <c r="C186" s="3"/>
@@ -6845,7 +6846,7 @@
       <c r="Y186" s="6"/>
       <c r="Z186" s="6"/>
     </row>
-    <row r="187" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:26" ht="12.75">
       <c r="A187" s="11"/>
       <c r="B187" s="2"/>
       <c r="C187" s="3"/>
@@ -6873,7 +6874,7 @@
       <c r="Y187" s="6"/>
       <c r="Z187" s="6"/>
     </row>
-    <row r="188" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:26" ht="12.75">
       <c r="A188" s="11"/>
       <c r="B188" s="2"/>
       <c r="C188" s="3"/>
@@ -6901,7 +6902,7 @@
       <c r="Y188" s="6"/>
       <c r="Z188" s="6"/>
     </row>
-    <row r="189" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:26" ht="12.75">
       <c r="A189" s="11"/>
       <c r="B189" s="2"/>
       <c r="C189" s="3"/>
@@ -6929,7 +6930,7 @@
       <c r="Y189" s="6"/>
       <c r="Z189" s="6"/>
     </row>
-    <row r="190" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:26" ht="12.75">
       <c r="A190" s="6"/>
       <c r="B190" s="6"/>
       <c r="C190" s="21"/>
@@ -6957,7 +6958,7 @@
       <c r="Y190" s="6"/>
       <c r="Z190" s="6"/>
     </row>
-    <row r="191" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:26" ht="15">
       <c r="A191" s="7"/>
       <c r="B191" s="2"/>
       <c r="C191" s="3"/>
@@ -6985,7 +6986,7 @@
       <c r="Y191" s="6"/>
       <c r="Z191" s="6"/>
     </row>
-    <row r="192" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:26" ht="15">
       <c r="A192" s="7"/>
       <c r="B192" s="2"/>
       <c r="C192" s="3"/>
@@ -7013,7 +7014,7 @@
       <c r="Y192" s="6"/>
       <c r="Z192" s="6"/>
     </row>
-    <row r="193" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:26" ht="12.75">
       <c r="A193" s="7"/>
       <c r="B193" s="2"/>
       <c r="C193" s="3"/>
@@ -7041,7 +7042,7 @@
       <c r="Y193" s="6"/>
       <c r="Z193" s="6"/>
     </row>
-    <row r="194" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:26" ht="12.75">
       <c r="A194" s="7"/>
       <c r="B194" s="2"/>
       <c r="C194" s="3"/>
@@ -7069,7 +7070,7 @@
       <c r="Y194" s="6"/>
       <c r="Z194" s="6"/>
     </row>
-    <row r="195" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:26" ht="12.75">
       <c r="A195" s="7"/>
       <c r="B195" s="2"/>
       <c r="C195" s="3"/>
@@ -7097,7 +7098,7 @@
       <c r="Y195" s="6"/>
       <c r="Z195" s="6"/>
     </row>
-    <row r="196" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:26" ht="12.75">
       <c r="A196" s="7"/>
       <c r="B196" s="2"/>
       <c r="C196" s="3"/>
@@ -7125,7 +7126,7 @@
       <c r="Y196" s="6"/>
       <c r="Z196" s="6"/>
     </row>
-    <row r="197" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:26" ht="12.75">
       <c r="A197" s="7"/>
       <c r="B197" s="2"/>
       <c r="C197" s="3"/>
@@ -7153,7 +7154,7 @@
       <c r="Y197" s="6"/>
       <c r="Z197" s="6"/>
     </row>
-    <row r="198" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:26" ht="15">
       <c r="A198" s="2"/>
       <c r="B198" s="2"/>
       <c r="C198" s="8"/>
@@ -7181,7 +7182,7 @@
       <c r="Y198" s="6"/>
       <c r="Z198" s="6"/>
     </row>
-    <row r="199" spans="1:26" ht="15" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:26" ht="15">
       <c r="A199" s="2"/>
       <c r="B199" s="2"/>
       <c r="C199" s="8"/>
@@ -7209,7 +7210,7 @@
       <c r="Y199" s="6"/>
       <c r="Z199" s="6"/>
     </row>
-    <row r="200" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:26" ht="12.75">
       <c r="A200" s="2"/>
       <c r="B200" s="2"/>
       <c r="C200" s="8"/>
@@ -7237,7 +7238,7 @@
       <c r="Y200" s="6"/>
       <c r="Z200" s="6"/>
     </row>
-    <row r="201" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:26" ht="12.75">
       <c r="A201" s="2"/>
       <c r="B201" s="2"/>
       <c r="C201" s="8"/>
@@ -7265,7 +7266,7 @@
       <c r="Y201" s="6"/>
       <c r="Z201" s="6"/>
     </row>
-    <row r="202" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:26" ht="12.75">
       <c r="A202" s="2"/>
       <c r="B202" s="2"/>
       <c r="C202" s="8"/>
@@ -7293,7 +7294,7 @@
       <c r="Y202" s="6"/>
       <c r="Z202" s="6"/>
     </row>
-    <row r="203" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:26" ht="12.75">
       <c r="A203" s="2"/>
       <c r="B203" s="2"/>
       <c r="C203" s="8"/>
@@ -7321,7 +7322,7 @@
       <c r="Y203" s="6"/>
       <c r="Z203" s="6"/>
     </row>
-    <row r="204" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:26" ht="12.75">
       <c r="A204" s="6"/>
       <c r="B204" s="6"/>
       <c r="C204" s="21"/>
@@ -7349,7 +7350,7 @@
       <c r="Y204" s="6"/>
       <c r="Z204" s="6"/>
     </row>
-    <row r="205" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:26" ht="12.75">
       <c r="A205" s="7"/>
       <c r="B205" s="2"/>
       <c r="C205" s="19"/>
@@ -7377,7 +7378,7 @@
       <c r="Y205" s="4"/>
       <c r="Z205" s="4"/>
     </row>
-    <row r="206" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:26" ht="12.75">
       <c r="A206" s="7"/>
       <c r="B206" s="2"/>
       <c r="C206" s="19"/>
@@ -7405,7 +7406,7 @@
       <c r="Y206" s="4"/>
       <c r="Z206" s="4"/>
     </row>
-    <row r="207" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:26" ht="12.75">
       <c r="A207" s="7"/>
       <c r="B207" s="2"/>
       <c r="C207" s="19"/>
@@ -7433,7 +7434,7 @@
       <c r="Y207" s="4"/>
       <c r="Z207" s="4"/>
     </row>
-    <row r="208" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:26" ht="12.75">
       <c r="A208" s="7"/>
       <c r="B208" s="2"/>
       <c r="C208" s="19"/>
@@ -7461,7 +7462,7 @@
       <c r="Y208" s="4"/>
       <c r="Z208" s="4"/>
     </row>
-    <row r="209" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:26" ht="12.75">
       <c r="A209" s="7"/>
       <c r="B209" s="2"/>
       <c r="C209" s="19"/>
@@ -7489,7 +7490,7 @@
       <c r="Y209" s="4"/>
       <c r="Z209" s="4"/>
     </row>
-    <row r="210" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:26" ht="12.75">
       <c r="A210" s="7"/>
       <c r="B210" s="2"/>
       <c r="C210" s="19"/>
@@ -7517,7 +7518,7 @@
       <c r="Y210" s="4"/>
       <c r="Z210" s="4"/>
     </row>
-    <row r="211" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:26" ht="12.75">
       <c r="A211" s="7"/>
       <c r="B211" s="2"/>
       <c r="C211" s="19"/>
@@ -7545,7 +7546,7 @@
       <c r="Y211" s="4"/>
       <c r="Z211" s="4"/>
     </row>
-    <row r="212" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:26" ht="12.75">
       <c r="A212" s="7"/>
       <c r="B212" s="2"/>
       <c r="C212" s="19"/>
@@ -7573,7 +7574,7 @@
       <c r="Y212" s="4"/>
       <c r="Z212" s="4"/>
     </row>
-    <row r="213" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:26" ht="12.75">
       <c r="A213" s="6"/>
       <c r="B213" s="6"/>
       <c r="C213" s="21"/>
@@ -7601,7 +7602,7 @@
       <c r="Y213" s="6"/>
       <c r="Z213" s="6"/>
     </row>
-    <row r="214" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:26" ht="12.75">
       <c r="A214" s="2"/>
       <c r="B214" s="33"/>
       <c r="C214" s="12"/>
@@ -7629,7 +7630,7 @@
       <c r="Y214" s="6"/>
       <c r="Z214" s="6"/>
     </row>
-    <row r="215" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:26" ht="12.75">
       <c r="A215" s="2"/>
       <c r="B215" s="33"/>
       <c r="C215" s="12"/>
@@ -7657,7 +7658,7 @@
       <c r="Y215" s="6"/>
       <c r="Z215" s="6"/>
     </row>
-    <row r="216" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:26" ht="12.75">
       <c r="A216" s="2"/>
       <c r="B216" s="33"/>
       <c r="C216" s="12"/>
@@ -7685,7 +7686,7 @@
       <c r="Y216" s="6"/>
       <c r="Z216" s="6"/>
     </row>
-    <row r="217" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:26" ht="12.75">
       <c r="A217" s="2"/>
       <c r="B217" s="33"/>
       <c r="C217" s="12"/>
@@ -7713,7 +7714,7 @@
       <c r="Y217" s="6"/>
       <c r="Z217" s="6"/>
     </row>
-    <row r="218" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:26" ht="12.75">
       <c r="A218" s="2"/>
       <c r="B218" s="33"/>
       <c r="C218" s="12"/>
@@ -7741,7 +7742,7 @@
       <c r="Y218" s="6"/>
       <c r="Z218" s="6"/>
     </row>
-    <row r="219" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:26" ht="12.75">
       <c r="A219" s="2"/>
       <c r="B219" s="33"/>
       <c r="C219" s="12"/>
@@ -7769,7 +7770,7 @@
       <c r="Y219" s="6"/>
       <c r="Z219" s="6"/>
     </row>
-    <row r="220" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:26" ht="12.75">
       <c r="A220" s="36"/>
       <c r="B220" s="37"/>
       <c r="C220" s="38"/>
@@ -7797,7 +7798,7 @@
       <c r="Y220" s="6"/>
       <c r="Z220" s="6"/>
     </row>
-    <row r="221" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:26" ht="12.75">
       <c r="A221" s="36"/>
       <c r="B221" s="40"/>
       <c r="C221" s="38"/>
@@ -7825,7 +7826,7 @@
       <c r="Y221" s="6"/>
       <c r="Z221" s="6"/>
     </row>
-    <row r="222" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:26" ht="12.75">
       <c r="A222" s="6"/>
       <c r="B222" s="6"/>
       <c r="C222" s="21"/>
@@ -7853,7 +7854,7 @@
       <c r="Y222" s="6"/>
       <c r="Z222" s="6"/>
     </row>
-    <row r="223" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:26" ht="12.75">
       <c r="A223" s="36"/>
       <c r="B223" s="36"/>
       <c r="C223" s="38"/>
@@ -7881,7 +7882,7 @@
       <c r="Y223" s="6"/>
       <c r="Z223" s="6"/>
     </row>
-    <row r="224" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:26" ht="12.75">
       <c r="A224" s="36"/>
       <c r="B224" s="36"/>
       <c r="C224" s="38"/>
@@ -7909,7 +7910,7 @@
       <c r="Y224" s="6"/>
       <c r="Z224" s="6"/>
     </row>
-    <row r="225" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:26" ht="12.75">
       <c r="A225" s="36"/>
       <c r="B225" s="36"/>
       <c r="C225" s="38"/>
@@ -7937,7 +7938,7 @@
       <c r="Y225" s="6"/>
       <c r="Z225" s="6"/>
     </row>
-    <row r="226" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:26" ht="12.75">
       <c r="A226" s="36"/>
       <c r="B226" s="36"/>
       <c r="C226" s="38"/>
@@ -7965,7 +7966,7 @@
       <c r="Y226" s="6"/>
       <c r="Z226" s="6"/>
     </row>
-    <row r="227" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:26" ht="12.75">
       <c r="A227" s="36"/>
       <c r="B227" s="36"/>
       <c r="C227" s="38"/>
@@ -7993,7 +7994,7 @@
       <c r="Y227" s="6"/>
       <c r="Z227" s="6"/>
     </row>
-    <row r="228" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:26" ht="12.75">
       <c r="A228" s="36"/>
       <c r="B228" s="36"/>
       <c r="C228" s="38"/>
@@ -8021,7 +8022,7 @@
       <c r="Y228" s="6"/>
       <c r="Z228" s="6"/>
     </row>
-    <row r="229" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:26" ht="12.75">
       <c r="A229" s="36"/>
       <c r="B229" s="36"/>
       <c r="C229" s="38"/>
@@ -8049,7 +8050,7 @@
       <c r="Y229" s="6"/>
       <c r="Z229" s="6"/>
     </row>
-    <row r="230" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:26" ht="12.75">
       <c r="A230" s="41"/>
       <c r="B230" s="41"/>
       <c r="C230" s="19"/>
@@ -8077,7 +8078,7 @@
       <c r="Y230" s="6"/>
       <c r="Z230" s="6"/>
     </row>
-    <row r="231" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:26" ht="12.75">
       <c r="A231" s="6"/>
       <c r="B231" s="6"/>
       <c r="C231" s="21"/>
@@ -8105,7 +8106,7 @@
       <c r="Y231" s="6"/>
       <c r="Z231" s="6"/>
     </row>
-    <row r="232" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:26" ht="12.75">
       <c r="A232" s="2"/>
       <c r="B232" s="33"/>
       <c r="C232" s="12"/>
@@ -8133,7 +8134,7 @@
       <c r="Y232" s="6"/>
       <c r="Z232" s="6"/>
     </row>
-    <row r="233" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:26" ht="12.75">
       <c r="A233" s="36"/>
       <c r="B233" s="40"/>
       <c r="C233" s="38"/>
@@ -8161,7 +8162,7 @@
       <c r="Y233" s="6"/>
       <c r="Z233" s="6"/>
     </row>
-    <row r="234" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:26" ht="12.75">
       <c r="A234" s="36"/>
       <c r="B234" s="40"/>
       <c r="C234" s="38"/>
@@ -8189,7 +8190,7 @@
       <c r="Y234" s="6"/>
       <c r="Z234" s="6"/>
     </row>
-    <row r="235" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:26" ht="12.75">
       <c r="A235" s="36"/>
       <c r="B235" s="40"/>
       <c r="C235" s="38"/>
@@ -8217,7 +8218,7 @@
       <c r="Y235" s="6"/>
       <c r="Z235" s="6"/>
     </row>
-    <row r="236" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:26" ht="12.75">
       <c r="A236" s="36"/>
       <c r="B236" s="40"/>
       <c r="C236" s="38"/>
@@ -8245,7 +8246,7 @@
       <c r="Y236" s="6"/>
       <c r="Z236" s="6"/>
     </row>
-    <row r="237" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:26" ht="12.75">
       <c r="A237" s="36"/>
       <c r="B237" s="40"/>
       <c r="C237" s="38"/>
@@ -8273,7 +8274,7 @@
       <c r="Y237" s="6"/>
       <c r="Z237" s="6"/>
     </row>
-    <row r="238" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:26" ht="12.75">
       <c r="A238" s="36"/>
       <c r="B238" s="40"/>
       <c r="C238" s="38"/>
@@ -8301,7 +8302,7 @@
       <c r="Y238" s="6"/>
       <c r="Z238" s="6"/>
     </row>
-    <row r="239" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:26" ht="12.75">
       <c r="A239" s="36"/>
       <c r="B239" s="40"/>
       <c r="C239" s="38"/>
@@ -8329,7 +8330,7 @@
       <c r="Y239" s="6"/>
       <c r="Z239" s="6"/>
     </row>
-    <row r="240" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:26" ht="12.75">
       <c r="A240" s="6"/>
       <c r="B240" s="6"/>
       <c r="C240" s="21"/>
@@ -8357,7 +8358,7 @@
       <c r="Y240" s="6"/>
       <c r="Z240" s="6"/>
     </row>
-    <row r="241" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:26" ht="12.75">
       <c r="A241" s="2"/>
       <c r="B241" s="33"/>
       <c r="C241" s="12"/>
@@ -8385,7 +8386,7 @@
       <c r="Y241" s="6"/>
       <c r="Z241" s="6"/>
     </row>
-    <row r="242" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:26" ht="12.75">
       <c r="A242" s="36"/>
       <c r="B242" s="40"/>
       <c r="C242" s="38"/>
@@ -8413,7 +8414,7 @@
       <c r="Y242" s="6"/>
       <c r="Z242" s="6"/>
     </row>
-    <row r="243" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:26" ht="12.75">
       <c r="A243" s="36"/>
       <c r="B243" s="40"/>
       <c r="C243" s="38"/>
@@ -8441,7 +8442,7 @@
       <c r="Y243" s="6"/>
       <c r="Z243" s="6"/>
     </row>
-    <row r="244" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:26" ht="12.75">
       <c r="A244" s="36"/>
       <c r="B244" s="40"/>
       <c r="C244" s="38"/>
@@ -8469,7 +8470,7 @@
       <c r="Y244" s="6"/>
       <c r="Z244" s="6"/>
     </row>
-    <row r="245" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:26" ht="12.75">
       <c r="A245" s="36"/>
       <c r="B245" s="40"/>
       <c r="C245" s="38"/>
@@ -8497,7 +8498,7 @@
       <c r="Y245" s="6"/>
       <c r="Z245" s="6"/>
     </row>
-    <row r="246" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:26" ht="12.75">
       <c r="A246" s="36"/>
       <c r="B246" s="40"/>
       <c r="C246" s="38"/>
@@ -8525,7 +8526,7 @@
       <c r="Y246" s="6"/>
       <c r="Z246" s="6"/>
     </row>
-    <row r="247" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:26" ht="12.75">
       <c r="A247" s="36"/>
       <c r="B247" s="40"/>
       <c r="C247" s="38"/>
@@ -8553,7 +8554,7 @@
       <c r="Y247" s="6"/>
       <c r="Z247" s="6"/>
     </row>
-    <row r="248" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:26" ht="12.75">
       <c r="A248" s="36"/>
       <c r="B248" s="40"/>
       <c r="C248" s="38"/>
@@ -8581,7 +8582,7 @@
       <c r="Y248" s="6"/>
       <c r="Z248" s="6"/>
     </row>
-    <row r="249" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:26" ht="12.75">
       <c r="A249" s="6"/>
       <c r="B249" s="6"/>
       <c r="C249" s="21"/>
@@ -8609,7 +8610,7 @@
       <c r="Y249" s="6"/>
       <c r="Z249" s="6"/>
     </row>
-    <row r="250" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:26" ht="12.75">
       <c r="A250" s="36"/>
       <c r="B250" s="40"/>
       <c r="C250" s="38"/>
@@ -8637,7 +8638,7 @@
       <c r="Y250" s="6"/>
       <c r="Z250" s="6"/>
     </row>
-    <row r="251" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:26" ht="12.75">
       <c r="A251" s="36"/>
       <c r="B251" s="40"/>
       <c r="C251" s="38"/>
@@ -8665,7 +8666,7 @@
       <c r="Y251" s="6"/>
       <c r="Z251" s="6"/>
     </row>
-    <row r="252" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:26" ht="12.75">
       <c r="A252" s="36"/>
       <c r="B252" s="40"/>
       <c r="C252" s="38"/>
@@ -8693,7 +8694,7 @@
       <c r="Y252" s="6"/>
       <c r="Z252" s="6"/>
     </row>
-    <row r="253" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:26" ht="12.75">
       <c r="A253" s="36"/>
       <c r="B253" s="40"/>
       <c r="C253" s="38"/>
@@ -8721,7 +8722,7 @@
       <c r="Y253" s="6"/>
       <c r="Z253" s="6"/>
     </row>
-    <row r="254" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:26" ht="12.75">
       <c r="A254" s="36"/>
       <c r="B254" s="40"/>
       <c r="C254" s="38"/>
@@ -8749,7 +8750,7 @@
       <c r="Y254" s="6"/>
       <c r="Z254" s="6"/>
     </row>
-    <row r="255" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:26" ht="12.75">
       <c r="A255" s="36"/>
       <c r="B255" s="40"/>
       <c r="C255" s="38"/>
@@ -8777,7 +8778,7 @@
       <c r="Y255" s="6"/>
       <c r="Z255" s="6"/>
     </row>
-    <row r="256" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:26" ht="12.75">
       <c r="A256" s="36"/>
       <c r="B256" s="40"/>
       <c r="C256" s="38"/>
@@ -8805,7 +8806,7 @@
       <c r="Y256" s="6"/>
       <c r="Z256" s="6"/>
     </row>
-    <row r="257" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:26" ht="12.75">
       <c r="A257" s="36"/>
       <c r="B257" s="40"/>
       <c r="C257" s="38"/>
@@ -8833,7 +8834,7 @@
       <c r="Y257" s="6"/>
       <c r="Z257" s="6"/>
     </row>
-    <row r="258" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:26" ht="12.75">
       <c r="A258" s="6"/>
       <c r="B258" s="6"/>
       <c r="C258" s="21"/>
@@ -8861,7 +8862,7 @@
       <c r="Y258" s="6"/>
       <c r="Z258" s="6"/>
     </row>
-    <row r="259" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:26" ht="12.75">
       <c r="A259" s="7"/>
       <c r="B259" s="2"/>
       <c r="C259" s="19"/>
@@ -8889,7 +8890,7 @@
       <c r="Y259" s="4"/>
       <c r="Z259" s="4"/>
     </row>
-    <row r="260" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:26" ht="12.75">
       <c r="A260" s="7"/>
       <c r="B260" s="2"/>
       <c r="C260" s="19"/>
@@ -8917,7 +8918,7 @@
       <c r="Y260" s="4"/>
       <c r="Z260" s="4"/>
     </row>
-    <row r="261" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:26" ht="12.75">
       <c r="A261" s="7"/>
       <c r="B261" s="2"/>
       <c r="C261" s="19"/>
@@ -8945,7 +8946,7 @@
       <c r="Y261" s="4"/>
       <c r="Z261" s="4"/>
     </row>
-    <row r="262" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:26" ht="12.75">
       <c r="A262" s="6"/>
       <c r="B262" s="6"/>
       <c r="C262" s="21"/>
@@ -8973,7 +8974,7 @@
       <c r="Y262" s="6"/>
       <c r="Z262" s="6"/>
     </row>
-    <row r="263" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:26" ht="12.75">
       <c r="A263" s="2"/>
       <c r="B263" s="7"/>
       <c r="C263" s="17"/>
@@ -9001,7 +9002,7 @@
       <c r="Y263" s="4"/>
       <c r="Z263" s="4"/>
     </row>
-    <row r="264" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:26" ht="12.75">
       <c r="A264" s="2"/>
       <c r="B264" s="7"/>
       <c r="C264" s="17"/>
@@ -9029,7 +9030,7 @@
       <c r="Y264" s="6"/>
       <c r="Z264" s="6"/>
     </row>
-    <row r="265" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:26" ht="12.75">
       <c r="A265" s="2"/>
       <c r="B265" s="7"/>
       <c r="C265" s="17"/>
@@ -9057,7 +9058,7 @@
       <c r="Y265" s="6"/>
       <c r="Z265" s="6"/>
     </row>
-    <row r="266" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:26" ht="12.75">
       <c r="A266" s="6"/>
       <c r="B266" s="6"/>
       <c r="C266" s="21"/>
@@ -9085,7 +9086,7 @@
       <c r="Y266" s="6"/>
       <c r="Z266" s="6"/>
     </row>
-    <row r="267" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:26" ht="12.75">
       <c r="A267" s="7"/>
       <c r="B267" s="10"/>
       <c r="C267" s="3"/>
@@ -9113,7 +9114,7 @@
       <c r="Y267" s="6"/>
       <c r="Z267" s="6"/>
     </row>
-    <row r="268" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:26" ht="12.75">
       <c r="A268" s="7"/>
       <c r="B268" s="10"/>
       <c r="C268" s="3"/>
@@ -9141,7 +9142,7 @@
       <c r="Y268" s="6"/>
       <c r="Z268" s="6"/>
     </row>
-    <row r="269" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:26" ht="12.75">
       <c r="A269" s="7"/>
       <c r="B269" s="10"/>
       <c r="C269" s="3"/>
@@ -9169,7 +9170,7 @@
       <c r="Y269" s="6"/>
       <c r="Z269" s="6"/>
     </row>
-    <row r="270" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:26" ht="12.75">
       <c r="A270" s="7"/>
       <c r="B270" s="10"/>
       <c r="C270" s="3"/>
@@ -9197,7 +9198,7 @@
       <c r="Y270" s="6"/>
       <c r="Z270" s="6"/>
     </row>
-    <row r="271" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:26" ht="12.75">
       <c r="A271" s="7"/>
       <c r="B271" s="10"/>
       <c r="C271" s="3"/>
@@ -9225,7 +9226,7 @@
       <c r="Y271" s="6"/>
       <c r="Z271" s="6"/>
     </row>
-    <row r="272" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:26" ht="12.75">
       <c r="A272" s="7"/>
       <c r="B272" s="10"/>
       <c r="C272" s="3"/>
@@ -9253,7 +9254,7 @@
       <c r="Y272" s="6"/>
       <c r="Z272" s="6"/>
     </row>
-    <row r="273" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:26" ht="12.75">
       <c r="A273" s="4"/>
       <c r="B273" s="4"/>
       <c r="C273" s="22"/>
@@ -9281,7 +9282,7 @@
       <c r="Y273" s="6"/>
       <c r="Z273" s="6"/>
     </row>
-    <row r="274" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:26" ht="12.75">
       <c r="A274" s="7"/>
       <c r="B274" s="2"/>
       <c r="C274" s="3"/>
@@ -9309,7 +9310,7 @@
       <c r="Y274" s="6"/>
       <c r="Z274" s="6"/>
     </row>
-    <row r="275" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:26" ht="12.75">
       <c r="A275" s="7"/>
       <c r="B275" s="2"/>
       <c r="C275" s="3"/>
@@ -9337,7 +9338,7 @@
       <c r="Y275" s="6"/>
       <c r="Z275" s="6"/>
     </row>
-    <row r="276" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:26" ht="12.75">
       <c r="A276" s="7"/>
       <c r="B276" s="2"/>
       <c r="C276" s="3"/>
@@ -9365,7 +9366,7 @@
       <c r="Y276" s="6"/>
       <c r="Z276" s="6"/>
     </row>
-    <row r="277" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:26" ht="12.75">
       <c r="A277" s="7"/>
       <c r="B277" s="2"/>
       <c r="C277" s="3"/>
@@ -9393,7 +9394,7 @@
       <c r="Y277" s="6"/>
       <c r="Z277" s="6"/>
     </row>
-    <row r="278" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:26" ht="12.75">
       <c r="A278" s="7"/>
       <c r="B278" s="2"/>
       <c r="C278" s="3"/>
@@ -9421,7 +9422,7 @@
       <c r="Y278" s="6"/>
       <c r="Z278" s="6"/>
     </row>
-    <row r="279" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:26" ht="12.75">
       <c r="A279" s="7"/>
       <c r="B279" s="2"/>
       <c r="C279" s="3"/>
@@ -9449,7 +9450,7 @@
       <c r="Y279" s="6"/>
       <c r="Z279" s="6"/>
     </row>
-    <row r="280" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:26" ht="12.75">
       <c r="A280" s="4"/>
       <c r="B280" s="4"/>
       <c r="C280" s="22"/>
@@ -9477,7 +9478,7 @@
       <c r="Y280" s="6"/>
       <c r="Z280" s="6"/>
     </row>
-    <row r="281" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:26" ht="12.75">
       <c r="A281" s="2"/>
       <c r="B281" s="2"/>
       <c r="C281" s="3"/>
@@ -9505,7 +9506,7 @@
       <c r="Y281" s="6"/>
       <c r="Z281" s="6"/>
     </row>
-    <row r="282" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:26" ht="12.75">
       <c r="A282" s="2"/>
       <c r="B282" s="2"/>
       <c r="C282" s="3"/>
@@ -9533,7 +9534,7 @@
       <c r="Y282" s="6"/>
       <c r="Z282" s="6"/>
     </row>
-    <row r="283" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:26" ht="12.75">
       <c r="A283" s="6"/>
       <c r="B283" s="2"/>
       <c r="C283" s="3"/>
@@ -9561,7 +9562,7 @@
       <c r="Y283" s="6"/>
       <c r="Z283" s="6"/>
     </row>
-    <row r="284" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:26" ht="12.75">
       <c r="A284" s="2"/>
       <c r="B284" s="2"/>
       <c r="C284" s="3"/>
@@ -9589,7 +9590,7 @@
       <c r="Y284" s="6"/>
       <c r="Z284" s="6"/>
     </row>
-    <row r="285" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:26" ht="12.75">
       <c r="A285" s="7"/>
       <c r="B285" s="2"/>
       <c r="C285" s="3"/>
@@ -9617,7 +9618,7 @@
       <c r="Y285" s="6"/>
       <c r="Z285" s="6"/>
     </row>
-    <row r="286" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:26" ht="12.75">
       <c r="A286" s="7"/>
       <c r="B286" s="2"/>
       <c r="C286" s="3"/>
@@ -9645,7 +9646,7 @@
       <c r="Y286" s="6"/>
       <c r="Z286" s="6"/>
     </row>
-    <row r="287" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:26" ht="12.75">
       <c r="A287" s="7"/>
       <c r="B287" s="2"/>
       <c r="C287" s="3"/>
@@ -9673,7 +9674,7 @@
       <c r="Y287" s="6"/>
       <c r="Z287" s="6"/>
     </row>
-    <row r="288" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:26" ht="12.75">
       <c r="A288" s="2"/>
       <c r="B288" s="2"/>
       <c r="C288" s="3"/>
@@ -9701,7 +9702,7 @@
       <c r="Y288" s="6"/>
       <c r="Z288" s="6"/>
     </row>
-    <row r="289" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:26" ht="12.75">
       <c r="A289" s="7"/>
       <c r="B289" s="2"/>
       <c r="C289" s="3"/>
@@ -9729,7 +9730,7 @@
       <c r="Y289" s="6"/>
       <c r="Z289" s="6"/>
     </row>
-    <row r="290" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:26" ht="12.75">
       <c r="A290" s="7"/>
       <c r="B290" s="2"/>
       <c r="C290" s="3"/>
@@ -9757,7 +9758,7 @@
       <c r="Y290" s="6"/>
       <c r="Z290" s="6"/>
     </row>
-    <row r="291" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:26" ht="12.75">
       <c r="A291" s="7"/>
       <c r="B291" s="2"/>
       <c r="C291" s="3"/>
@@ -9785,7 +9786,7 @@
       <c r="Y291" s="6"/>
       <c r="Z291" s="6"/>
     </row>
-    <row r="292" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:26" ht="12.75">
       <c r="A292" s="7"/>
       <c r="B292" s="2"/>
       <c r="C292" s="3"/>
@@ -9813,7 +9814,7 @@
       <c r="Y292" s="6"/>
       <c r="Z292" s="6"/>
     </row>
-    <row r="293" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:26" ht="12.75">
       <c r="A293" s="7"/>
       <c r="B293" s="2"/>
       <c r="C293" s="3"/>
@@ -9841,7 +9842,7 @@
       <c r="Y293" s="6"/>
       <c r="Z293" s="6"/>
     </row>
-    <row r="294" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:26" ht="12.75">
       <c r="A294" s="7"/>
       <c r="B294" s="2"/>
       <c r="C294" s="3"/>
@@ -9869,7 +9870,7 @@
       <c r="Y294" s="6"/>
       <c r="Z294" s="6"/>
     </row>
-    <row r="295" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:26" ht="12.75">
       <c r="A295" s="7"/>
       <c r="B295" s="2"/>
       <c r="C295" s="3"/>
@@ -9897,7 +9898,7 @@
       <c r="Y295" s="6"/>
       <c r="Z295" s="6"/>
     </row>
-    <row r="296" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:26" ht="12.75">
       <c r="A296" s="7"/>
       <c r="B296" s="2"/>
       <c r="C296" s="3"/>
@@ -9925,7 +9926,7 @@
       <c r="Y296" s="6"/>
       <c r="Z296" s="6"/>
     </row>
-    <row r="297" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:26" ht="12.75">
       <c r="A297" s="7"/>
       <c r="B297" s="2"/>
       <c r="C297" s="3"/>
@@ -9953,7 +9954,7 @@
       <c r="Y297" s="6"/>
       <c r="Z297" s="6"/>
     </row>
-    <row r="298" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:26" ht="12.75">
       <c r="A298" s="7"/>
       <c r="B298" s="2"/>
       <c r="C298" s="3"/>
@@ -9981,7 +9982,7 @@
       <c r="Y298" s="6"/>
       <c r="Z298" s="6"/>
     </row>
-    <row r="299" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:26" ht="12.75">
       <c r="A299" s="7"/>
       <c r="B299" s="2"/>
       <c r="C299" s="3"/>
@@ -10009,7 +10010,7 @@
       <c r="Y299" s="6"/>
       <c r="Z299" s="6"/>
     </row>
-    <row r="300" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:26" ht="12.75">
       <c r="A300" s="7"/>
       <c r="B300" s="2"/>
       <c r="C300" s="3"/>
@@ -10037,7 +10038,7 @@
       <c r="Y300" s="6"/>
       <c r="Z300" s="6"/>
     </row>
-    <row r="301" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:26" ht="12.75">
       <c r="A301" s="7"/>
       <c r="B301" s="2"/>
       <c r="C301" s="3"/>
@@ -10065,7 +10066,7 @@
       <c r="Y301" s="6"/>
       <c r="Z301" s="6"/>
     </row>
-    <row r="302" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:26" ht="12.75">
       <c r="A302" s="4"/>
       <c r="B302" s="23"/>
       <c r="C302" s="24"/>
@@ -10093,7 +10094,7 @@
       <c r="Y302" s="6"/>
       <c r="Z302" s="6"/>
     </row>
-    <row r="303" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:26" ht="12.75">
       <c r="A303" s="2"/>
       <c r="B303" s="23"/>
       <c r="C303" s="24"/>
@@ -10121,7 +10122,7 @@
       <c r="Y303" s="6"/>
       <c r="Z303" s="6"/>
     </row>
-    <row r="304" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:26" ht="12.75">
       <c r="A304" s="2"/>
       <c r="B304" s="6"/>
       <c r="C304" s="21"/>
@@ -10149,7 +10150,7 @@
       <c r="Y304" s="6"/>
       <c r="Z304" s="6"/>
     </row>
-    <row r="305" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:26" ht="12.75">
       <c r="A305" s="2"/>
       <c r="B305" s="6"/>
       <c r="C305" s="21"/>
@@ -10177,7 +10178,7 @@
       <c r="Y305" s="6"/>
       <c r="Z305" s="6"/>
     </row>
-    <row r="306" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:26" ht="12.75">
       <c r="A306" s="2"/>
       <c r="B306" s="6"/>
       <c r="C306" s="21"/>
@@ -10205,7 +10206,7 @@
       <c r="Y306" s="6"/>
       <c r="Z306" s="6"/>
     </row>
-    <row r="307" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:26" ht="12.75">
       <c r="A307" s="2"/>
       <c r="B307" s="6"/>
       <c r="C307" s="21"/>
@@ -10233,7 +10234,7 @@
       <c r="Y307" s="6"/>
       <c r="Z307" s="6"/>
     </row>
-    <row r="308" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:26" ht="12.75">
       <c r="A308" s="2"/>
       <c r="B308" s="6"/>
       <c r="C308" s="21"/>
@@ -10261,7 +10262,7 @@
       <c r="Y308" s="6"/>
       <c r="Z308" s="6"/>
     </row>
-    <row r="309" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:26" ht="12.75">
       <c r="A309" s="2"/>
       <c r="B309" s="6"/>
       <c r="C309" s="21"/>
@@ -10289,7 +10290,7 @@
       <c r="Y309" s="6"/>
       <c r="Z309" s="6"/>
     </row>
-    <row r="310" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:26" ht="12.75">
       <c r="A310" s="2"/>
       <c r="B310" s="6"/>
       <c r="C310" s="21"/>
@@ -10317,7 +10318,7 @@
       <c r="Y310" s="6"/>
       <c r="Z310" s="6"/>
     </row>
-    <row r="311" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:26" ht="12.75">
       <c r="A311" s="2"/>
       <c r="B311" s="6"/>
       <c r="C311" s="21"/>
@@ -10345,7 +10346,7 @@
       <c r="Y311" s="6"/>
       <c r="Z311" s="6"/>
     </row>
-    <row r="312" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:26" ht="12.75">
       <c r="A312" s="2"/>
       <c r="B312" s="6"/>
       <c r="C312" s="21"/>
@@ -10373,7 +10374,7 @@
       <c r="Y312" s="6"/>
       <c r="Z312" s="6"/>
     </row>
-    <row r="313" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:26" ht="12.75">
       <c r="A313" s="2"/>
       <c r="B313" s="6"/>
       <c r="C313" s="21"/>
@@ -10401,7 +10402,7 @@
       <c r="Y313" s="6"/>
       <c r="Z313" s="6"/>
     </row>
-    <row r="314" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:26" ht="12.75">
       <c r="A314" s="2"/>
       <c r="B314" s="6"/>
       <c r="C314" s="21"/>
@@ -10429,7 +10430,7 @@
       <c r="Y314" s="6"/>
       <c r="Z314" s="6"/>
     </row>
-    <row r="315" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:26" ht="12.75">
       <c r="A315" s="6"/>
       <c r="B315" s="6"/>
       <c r="C315" s="21"/>
@@ -10457,7 +10458,7 @@
       <c r="Y315" s="6"/>
       <c r="Z315" s="6"/>
     </row>
-    <row r="316" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:26" ht="12.75">
       <c r="A316" s="6"/>
       <c r="B316" s="6"/>
       <c r="C316" s="21"/>
@@ -10485,7 +10486,7 @@
       <c r="Y316" s="6"/>
       <c r="Z316" s="6"/>
     </row>
-    <row r="317" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:26" ht="12.75">
       <c r="A317" s="6"/>
       <c r="B317" s="6"/>
       <c r="C317" s="21"/>
@@ -10513,7 +10514,7 @@
       <c r="Y317" s="6"/>
       <c r="Z317" s="6"/>
     </row>
-    <row r="318" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:26" ht="12.75">
       <c r="A318" s="6"/>
       <c r="B318" s="6"/>
       <c r="C318" s="21"/>
@@ -10541,7 +10542,7 @@
       <c r="Y318" s="6"/>
       <c r="Z318" s="6"/>
     </row>
-    <row r="319" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:26" ht="12.75">
       <c r="A319" s="2"/>
       <c r="B319" s="6"/>
       <c r="C319" s="21"/>
@@ -10569,7 +10570,7 @@
       <c r="Y319" s="6"/>
       <c r="Z319" s="6"/>
     </row>
-    <row r="320" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:26" ht="12.75">
       <c r="A320" s="6"/>
       <c r="B320" s="6"/>
       <c r="C320" s="21"/>
@@ -10597,7 +10598,7 @@
       <c r="Y320" s="6"/>
       <c r="Z320" s="6"/>
     </row>
-    <row r="321" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:26" ht="12.75">
       <c r="A321" s="6"/>
       <c r="B321" s="6"/>
       <c r="C321" s="21"/>
@@ -10625,7 +10626,7 @@
       <c r="Y321" s="6"/>
       <c r="Z321" s="6"/>
     </row>
-    <row r="322" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:26" ht="12.75">
       <c r="A322" s="6"/>
       <c r="B322" s="6"/>
       <c r="C322" s="21"/>
@@ -10653,7 +10654,7 @@
       <c r="Y322" s="6"/>
       <c r="Z322" s="6"/>
     </row>
-    <row r="323" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:26" ht="12.75">
       <c r="A323" s="6"/>
       <c r="B323" s="6"/>
       <c r="C323" s="21"/>
@@ -10681,7 +10682,7 @@
       <c r="Y323" s="6"/>
       <c r="Z323" s="6"/>
     </row>
-    <row r="324" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:26" ht="12.75">
       <c r="A324" s="6"/>
       <c r="B324" s="6"/>
       <c r="C324" s="21"/>
@@ -10709,7 +10710,7 @@
       <c r="Y324" s="6"/>
       <c r="Z324" s="6"/>
     </row>
-    <row r="325" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:26" ht="12.75">
       <c r="A325" s="6"/>
       <c r="B325" s="6"/>
       <c r="C325" s="21"/>
@@ -10737,7 +10738,7 @@
       <c r="Y325" s="6"/>
       <c r="Z325" s="6"/>
     </row>
-    <row r="326" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:26" ht="12.75">
       <c r="A326" s="2"/>
       <c r="B326" s="6"/>
       <c r="C326" s="21"/>
@@ -10765,7 +10766,7 @@
       <c r="Y326" s="6"/>
       <c r="Z326" s="6"/>
     </row>
-    <row r="327" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:26" ht="12.75">
       <c r="A327" s="2"/>
       <c r="B327" s="6"/>
       <c r="C327" s="21"/>
@@ -10793,7 +10794,7 @@
       <c r="Y327" s="6"/>
       <c r="Z327" s="6"/>
     </row>
-    <row r="328" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:26" ht="12.75">
       <c r="A328" s="2"/>
       <c r="B328" s="6"/>
       <c r="C328" s="21"/>
@@ -10821,7 +10822,7 @@
       <c r="Y328" s="6"/>
       <c r="Z328" s="6"/>
     </row>
-    <row r="329" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:26" ht="12.75">
       <c r="A329" s="2"/>
       <c r="B329" s="6"/>
       <c r="C329" s="21"/>
@@ -10849,7 +10850,7 @@
       <c r="Y329" s="6"/>
       <c r="Z329" s="6"/>
     </row>
-    <row r="330" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:26" ht="12.75">
       <c r="A330" s="2"/>
       <c r="B330" s="6"/>
       <c r="C330" s="21"/>
@@ -10877,7 +10878,7 @@
       <c r="Y330" s="6"/>
       <c r="Z330" s="6"/>
     </row>
-    <row r="331" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:26" ht="12.75">
       <c r="A331" s="2"/>
       <c r="B331" s="6"/>
       <c r="C331" s="21"/>
@@ -10905,7 +10906,7 @@
       <c r="Y331" s="6"/>
       <c r="Z331" s="6"/>
     </row>
-    <row r="332" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:26" ht="12.75">
       <c r="A332" s="2"/>
       <c r="B332" s="6"/>
       <c r="C332" s="21"/>
@@ -10933,7 +10934,7 @@
       <c r="Y332" s="6"/>
       <c r="Z332" s="6"/>
     </row>
-    <row r="333" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:26" ht="12.75">
       <c r="A333" s="6"/>
       <c r="B333" s="6"/>
       <c r="C333" s="21"/>
@@ -10961,7 +10962,7 @@
       <c r="Y333" s="6"/>
       <c r="Z333" s="6"/>
     </row>
-    <row r="334" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:26" ht="12.75">
       <c r="A334" s="2"/>
       <c r="B334" s="6"/>
       <c r="C334" s="21"/>
@@ -10996,20 +10997,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AM83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:AM83"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="25" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="26" max="38" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:39" ht="15">
       <c r="A1" s="107">
         <v>-5.1410999999999998E-2</v>
       </c>
@@ -11128,7 +11129,7 @@
         <v>1.4474000000000001E-2</v>
       </c>
     </row>
-    <row r="2" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:39" ht="15">
       <c r="A2" s="107">
         <v>-5.2628000000000001E-2</v>
       </c>
@@ -11247,7 +11248,7 @@
         <v>1.5002E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:39" ht="15">
       <c r="A3" s="107">
         <v>-5.3527999999999999E-2</v>
       </c>
@@ -11366,7 +11367,7 @@
         <v>1.6670000000000001E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:39" ht="15">
       <c r="A4" s="107">
         <v>-5.3511000000000003E-2</v>
       </c>
@@ -11485,7 +11486,7 @@
         <v>1.7100000000000001E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:39" ht="15">
       <c r="A5" s="107">
         <v>-5.1874999999999998E-2</v>
       </c>
@@ -11604,7 +11605,7 @@
         <v>1.6663000000000001E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:39" ht="15">
       <c r="A6" s="107">
         <v>-5.2708999999999999E-2</v>
       </c>
@@ -11723,7 +11724,7 @@
         <v>1.6922E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:39" ht="15">
       <c r="A7" s="107">
         <v>-4.9339000000000001E-2</v>
       </c>
@@ -11842,7 +11843,7 @@
         <v>1.7214E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:39" ht="15">
       <c r="A8" s="107">
         <v>-4.8416000000000001E-2</v>
       </c>
@@ -11961,7 +11962,7 @@
         <v>1.6704E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:39" ht="15">
       <c r="A9" s="107">
         <v>-4.7210000000000002E-2</v>
       </c>
@@ -12080,7 +12081,7 @@
         <v>1.6795999999999998E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:39" ht="15">
       <c r="A10" s="107">
         <v>-4.4845000000000003E-2</v>
       </c>
@@ -12199,7 +12200,7 @@
         <v>1.6015000000000001E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:39" ht="15">
       <c r="A11" s="107">
         <v>-4.4213000000000002E-2</v>
       </c>
@@ -12318,7 +12319,7 @@
         <v>1.5689999999999999E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:39" ht="15">
       <c r="A12" s="107">
         <v>-4.1450000000000001E-2</v>
       </c>
@@ -12437,7 +12438,7 @@
         <v>1.5408E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:39" ht="15">
       <c r="A13" s="107">
         <v>-0.04</v>
       </c>
@@ -12556,7 +12557,7 @@
         <v>1.4881E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:39" ht="15">
       <c r="A14" s="107">
         <v>-3.9252000000000002E-2</v>
       </c>
@@ -12675,7 +12676,7 @@
         <v>1.4279999999999999E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:39" ht="15">
       <c r="A15" s="107">
         <v>-3.6485999999999998E-2</v>
       </c>
@@ -12794,7 +12795,7 @@
         <v>1.3997000000000001E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:39" ht="15">
       <c r="A16" s="107">
         <v>-3.4934E-2</v>
       </c>
@@ -12913,7 +12914,7 @@
         <v>1.3191E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:39" ht="15">
       <c r="A17" s="107">
         <v>-3.3471000000000001E-2</v>
       </c>
@@ -13032,7 +13033,7 @@
         <v>1.2664999999999999E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:39" ht="15">
       <c r="A18" s="107">
         <v>-3.0973000000000001E-2</v>
       </c>
@@ -13151,7 +13152,7 @@
         <v>1.1899E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:39" ht="15">
       <c r="A19" s="107">
         <v>-3.0370000000000001E-2</v>
       </c>
@@ -13270,7 +13271,7 @@
         <v>1.1443999999999999E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:39" ht="15">
       <c r="A20" s="107">
         <v>-2.8670000000000001E-2</v>
       </c>
@@ -13389,7 +13390,7 @@
         <v>1.1010000000000001E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:39" ht="15">
       <c r="A21" s="107">
         <v>-2.7008000000000001E-2</v>
       </c>
@@ -13508,7 +13509,7 @@
         <v>1.0425E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:39" ht="15">
       <c r="A22" s="107">
         <v>-2.6433000000000002E-2</v>
       </c>
@@ -13627,7 +13628,7 @@
         <v>9.979E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:39" ht="15">
       <c r="A23" s="107">
         <v>-2.4525999999999999E-2</v>
       </c>
@@ -13746,7 +13747,7 @@
         <v>9.5219999999999992E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:39" ht="15">
       <c r="A24" s="107">
         <v>-2.3678000000000001E-2</v>
       </c>
@@ -13865,7 +13866,7 @@
         <v>9.0699999999999999E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:39" ht="15">
       <c r="A25" s="107">
         <v>-2.2699E-2</v>
       </c>
@@ -13984,7 +13985,7 @@
         <v>8.5419999999999992E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:39" ht="15">
       <c r="A26" s="107">
         <v>-2.0893999999999999E-2</v>
       </c>
@@ -14103,7 +14104,7 @@
         <v>8.2050000000000005E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:39" ht="15">
       <c r="A27" s="107">
         <v>-2.0428999999999999E-2</v>
       </c>
@@ -14222,7 +14223,7 @@
         <v>7.6860000000000001E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:39" ht="15">
       <c r="A28" s="107">
         <v>-1.9061999999999999E-2</v>
       </c>
@@ -14341,7 +14342,7 @@
         <v>7.4149999999999997E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:39" ht="15">
       <c r="A29" s="107">
         <v>-1.7776E-2</v>
       </c>
@@ -14460,7 +14461,7 @@
         <v>6.9719999999999999E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:39" ht="15">
       <c r="A30" s="107">
         <v>-1.7346E-2</v>
       </c>
@@ -14579,7 +14580,7 @@
         <v>6.5370000000000003E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:39" ht="15">
       <c r="A31" s="107">
         <v>-1.6291E-2</v>
       </c>
@@ -14698,7 +14699,7 @@
         <v>6.3569999999999998E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:39" ht="15">
       <c r="A32" s="107">
         <v>-1.5122E-2</v>
       </c>
@@ -14817,7 +14818,7 @@
         <v>6.0309999999999999E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:39" ht="15">
       <c r="A33" s="107">
         <v>-1.4371E-2</v>
       </c>
@@ -14936,7 +14937,7 @@
         <v>5.6889999999999996E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:39" ht="15">
       <c r="A34" s="107">
         <v>-1.2937000000000001E-2</v>
       </c>
@@ -15055,7 +15056,7 @@
         <v>5.5319999999999996E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:39" ht="15">
       <c r="A35" s="107">
         <v>-1.24E-2</v>
       </c>
@@ -15174,7 +15175,7 @@
         <v>5.3299999999999997E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:39" ht="15">
       <c r="A36" s="107">
         <v>-1.1819E-2</v>
       </c>
@@ -15293,7 +15294,7 @@
         <v>5.3150000000000003E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:39" ht="15">
       <c r="A37" s="107">
         <v>-1.1013E-2</v>
       </c>
@@ -15412,7 +15413,7 @@
         <v>5.3959999999999998E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:39" ht="15">
       <c r="A38" s="107">
         <v>-1.0744E-2</v>
       </c>
@@ -15531,7 +15532,7 @@
         <v>5.2230000000000002E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:39" ht="15">
       <c r="A39" s="107">
         <v>-1.0274999999999999E-2</v>
       </c>
@@ -15650,7 +15651,7 @@
         <v>5.306E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:39" ht="15">
       <c r="A40" s="107">
         <v>-9.9000000000000008E-3</v>
       </c>
@@ -15769,7 +15770,7 @@
         <v>5.2969999999999996E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:39" ht="15">
       <c r="A41" s="107">
         <v>-9.7009999999999996E-3</v>
       </c>
@@ -15888,7 +15889,7 @@
         <v>5.2189999999999997E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:39" ht="15">
       <c r="A42" s="107">
         <v>-9.3860000000000002E-3</v>
       </c>
@@ -16007,7 +16008,7 @@
         <v>5.2649999999999997E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:39" ht="15">
       <c r="A43" s="107">
         <v>-9.2820000000000003E-3</v>
       </c>
@@ -16126,7 +16127,7 @@
         <v>5.2249999999999996E-3</v>
       </c>
     </row>
-    <row r="44" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:39" ht="15">
       <c r="A44" s="107">
         <v>-9.7970000000000002E-3</v>
       </c>
@@ -16245,7 +16246,7 @@
         <v>5.0809999999999996E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:39" ht="15">
       <c r="A45" s="107">
         <v>-9.1039999999999992E-3</v>
       </c>
@@ -16364,7 +16365,7 @@
         <v>5.4270000000000004E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:39" ht="15">
       <c r="A46" s="107">
         <v>-8.4239999999999992E-3</v>
       </c>
@@ -16483,7 +16484,7 @@
         <v>5.4929999999999996E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:39" ht="15">
       <c r="A47" s="107">
         <v>-8.0479999999999996E-3</v>
       </c>
@@ -16602,7 +16603,7 @@
         <v>5.4130000000000003E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:39" ht="15">
       <c r="A48" s="107">
         <v>-8.038E-3</v>
       </c>
@@ -16721,7 +16722,7 @@
         <v>5.3299999999999997E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:39" ht="15">
       <c r="A49" s="107">
         <v>-7.5319999999999996E-3</v>
       </c>
@@ -16840,7 +16841,7 @@
         <v>5.2500000000000003E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:39" ht="15">
       <c r="A50" s="107">
         <v>-7.2639999999999996E-3</v>
       </c>
@@ -16959,7 +16960,7 @@
         <v>5.2180000000000004E-3</v>
       </c>
     </row>
-    <row r="51" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:39" ht="15">
       <c r="A51" s="107">
         <v>-6.973E-3</v>
       </c>
@@ -17078,7 +17079,7 @@
         <v>5.0569999999999999E-3</v>
       </c>
     </row>
-    <row r="52" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:39" ht="15">
       <c r="A52" s="107">
         <v>-6.548E-3</v>
       </c>
@@ -17197,7 +17198,7 @@
         <v>4.9119999999999997E-3</v>
       </c>
     </row>
-    <row r="53" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:39" ht="15">
       <c r="A53" s="107">
         <v>-6.3819999999999997E-3</v>
       </c>
@@ -17316,7 +17317,7 @@
         <v>4.7070000000000002E-3</v>
       </c>
     </row>
-    <row r="54" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:39" ht="15">
       <c r="A54" s="107">
         <v>-6.0559999999999998E-3</v>
       </c>
@@ -17435,7 +17436,7 @@
         <v>4.5950000000000001E-3</v>
       </c>
     </row>
-    <row r="55" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:39" ht="15">
       <c r="A55" s="107">
         <v>-5.8430000000000001E-3</v>
       </c>
@@ -17554,7 +17555,7 @@
         <v>4.444E-3</v>
       </c>
     </row>
-    <row r="56" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:39" ht="15">
       <c r="A56" s="107">
         <v>-5.5469999999999998E-3</v>
       </c>
@@ -17673,7 +17674,7 @@
         <v>4.3439999999999998E-3</v>
       </c>
     </row>
-    <row r="57" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:39" ht="15">
       <c r="A57" s="107">
         <v>-5.3969999999999999E-3</v>
       </c>
@@ -17792,7 +17793,7 @@
         <v>4.0670000000000003E-3</v>
       </c>
     </row>
-    <row r="58" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:39" ht="15">
       <c r="A58" s="107">
         <v>-5.2490000000000002E-3</v>
       </c>
@@ -17911,7 +17912,7 @@
         <v>3.954E-3</v>
       </c>
     </row>
-    <row r="59" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:39" ht="15">
       <c r="A59" s="107">
         <v>-4.9909999999999998E-3</v>
       </c>
@@ -18030,7 +18031,7 @@
         <v>3.8289999999999999E-3</v>
       </c>
     </row>
-    <row r="60" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:39" ht="15">
       <c r="A60" s="107">
         <v>-4.8440000000000002E-3</v>
       </c>
@@ -18149,7 +18150,7 @@
         <v>3.7160000000000001E-3</v>
       </c>
     </row>
-    <row r="61" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:39" ht="15">
       <c r="A61" s="107">
         <v>-4.7609999999999996E-3</v>
       </c>
@@ -18268,7 +18269,7 @@
         <v>3.5019999999999999E-3</v>
       </c>
     </row>
-    <row r="62" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:39" ht="15">
       <c r="A62" s="107">
         <v>-4.4949999999999999E-3</v>
       </c>
@@ -18387,7 +18388,7 @@
         <v>3.3240000000000001E-3</v>
       </c>
     </row>
-    <row r="63" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:39" ht="15">
       <c r="A63" s="107">
         <v>-4.235E-3</v>
       </c>
@@ -18506,7 +18507,7 @@
         <v>3.2330000000000002E-3</v>
       </c>
     </row>
-    <row r="64" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:39" ht="15">
       <c r="A64" s="107">
         <v>-4.0889999999999998E-3</v>
       </c>
@@ -18625,7 +18626,7 @@
         <v>3.0409999999999999E-3</v>
       </c>
     </row>
-    <row r="65" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:39" ht="15">
       <c r="A65" s="107">
         <v>-3.9830000000000004E-3</v>
       </c>
@@ -18744,7 +18745,7 @@
         <v>2.8029999999999999E-3</v>
       </c>
     </row>
-    <row r="66" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:39" ht="15">
       <c r="A66" s="107">
         <v>-3.6470000000000001E-3</v>
       </c>
@@ -18863,7 +18864,7 @@
         <v>2.66E-3</v>
       </c>
     </row>
-    <row r="67" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:39" ht="15">
       <c r="A67" s="107">
         <v>-3.4589999999999998E-3</v>
       </c>
@@ -18982,7 +18983,7 @@
         <v>2.4480000000000001E-3</v>
       </c>
     </row>
-    <row r="68" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:39" ht="15">
       <c r="A68" s="107">
         <v>-3.261E-3</v>
       </c>
@@ -19101,7 +19102,7 @@
         <v>2.2330000000000002E-3</v>
       </c>
     </row>
-    <row r="69" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:39" ht="15">
       <c r="A69" s="107">
         <v>-2.506E-3</v>
       </c>
@@ -19220,7 +19221,7 @@
         <v>1.9970000000000001E-3</v>
       </c>
     </row>
-    <row r="70" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:39" ht="15">
       <c r="A70" s="107">
         <v>-2.4529999999999999E-3</v>
       </c>
@@ -19339,7 +19340,7 @@
         <v>1.8209999999999999E-3</v>
       </c>
     </row>
-    <row r="71" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:39" ht="15">
       <c r="A71" s="107">
         <v>-2.1020000000000001E-3</v>
       </c>
@@ -19458,7 +19459,7 @@
         <v>1.6930000000000001E-3</v>
       </c>
     </row>
-    <row r="72" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:39" ht="15">
       <c r="A72" s="107">
         <v>-1.3990000000000001E-3</v>
       </c>
@@ -19577,7 +19578,7 @@
         <v>1.503E-3</v>
       </c>
     </row>
-    <row r="73" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:39" ht="15">
       <c r="A73" s="107">
         <v>-1.621E-3</v>
       </c>
@@ -19696,7 +19697,7 @@
         <v>1.482E-3</v>
       </c>
     </row>
-    <row r="74" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:39" ht="15">
       <c r="A74" s="107">
         <v>-1.1199999999999999E-3</v>
       </c>
@@ -19815,7 +19816,7 @@
         <v>1.488E-3</v>
       </c>
     </row>
-    <row r="75" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:39" ht="15">
       <c r="A75" s="107">
         <v>-9.5699999999999995E-4</v>
       </c>
@@ -19934,7 +19935,7 @@
         <v>1.5089999999999999E-3</v>
       </c>
     </row>
-    <row r="76" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:39" ht="15">
       <c r="A76" s="107">
         <v>-1.4859999999999999E-3</v>
       </c>
@@ -20053,7 +20054,7 @@
         <v>1.5629999999999999E-3</v>
       </c>
     </row>
-    <row r="77" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:39" ht="15">
       <c r="A77" s="107">
         <v>-3.6299999999999999E-4</v>
       </c>
@@ -20172,7 +20173,7 @@
         <v>1.5950000000000001E-3</v>
       </c>
     </row>
-    <row r="78" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:39" ht="15">
       <c r="A78" s="107">
         <v>-9.4399999999999996E-4</v>
       </c>
@@ -20291,7 +20292,7 @@
         <v>1.6100000000000001E-3</v>
       </c>
     </row>
-    <row r="79" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:39" ht="15">
       <c r="A79" s="107">
         <v>-1.24E-3</v>
       </c>
@@ -20410,7 +20411,7 @@
         <v>1.7129999999999999E-3</v>
       </c>
     </row>
-    <row r="80" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:39" ht="15">
       <c r="A80" s="107">
         <v>-3.9399999999999998E-4</v>
       </c>
@@ -20529,7 +20530,7 @@
         <v>1.7600000000000001E-3</v>
       </c>
     </row>
-    <row r="81" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:39" ht="15">
       <c r="A81" s="107">
         <v>-1.2999999999999999E-3</v>
       </c>
@@ -20648,7 +20649,7 @@
         <v>1.7390000000000001E-3</v>
       </c>
     </row>
-    <row r="82" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:39" ht="15">
       <c r="A82" s="107">
         <v>-1.8680000000000001E-3</v>
       </c>
@@ -20767,7 +20768,7 @@
         <v>1.6360000000000001E-3</v>
       </c>
     </row>
-    <row r="83" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:39" ht="15">
       <c r="A83" s="107">
         <v>-2.8410000000000002E-3</v>
       </c>
@@ -20892,21 +20893,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AM83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:AM83"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="24" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="25" max="26" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="27" max="37" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:39" ht="15">
       <c r="A1" s="107">
         <v>-3.7462000000000002E-2</v>
       </c>
@@ -21025,7 +21026,7 @@
         <v>-1.4499999999999999E-3</v>
       </c>
     </row>
-    <row r="2" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:39" ht="15">
       <c r="A2" s="107">
         <v>-3.6052000000000001E-2</v>
       </c>
@@ -21144,7 +21145,7 @@
         <v>-1.519E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:39" ht="15">
       <c r="A3" s="107">
         <v>-3.3577000000000003E-2</v>
       </c>
@@ -21263,7 +21264,7 @@
         <v>-3.6110000000000001E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:39" ht="15">
       <c r="A4" s="107">
         <v>-2.844E-2</v>
       </c>
@@ -21382,7 +21383,7 @@
         <v>-6.2129999999999998E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:39" ht="15">
       <c r="A5" s="107">
         <v>-2.2744E-2</v>
       </c>
@@ -21501,7 +21502,7 @@
         <v>-7.8079999999999998E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:39" ht="15">
       <c r="A6" s="107">
         <v>-1.8880000000000001E-2</v>
       </c>
@@ -21620,7 +21621,7 @@
         <v>-9.2180000000000005E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:39" ht="15">
       <c r="A7" s="107">
         <v>-1.541E-2</v>
       </c>
@@ -21739,7 +21740,7 @@
         <v>-9.8180000000000003E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:39" ht="15">
       <c r="A8" s="107">
         <v>-1.2751999999999999E-2</v>
       </c>
@@ -21858,7 +21859,7 @@
         <v>-9.8399999999999998E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:39" ht="15">
       <c r="A9" s="107">
         <v>-1.1493E-2</v>
       </c>
@@ -21977,7 +21978,7 @@
         <v>-9.306E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:39" ht="15">
       <c r="A10" s="107">
         <v>-1.0059E-2</v>
       </c>
@@ -22096,7 +22097,7 @@
         <v>-8.7180000000000001E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:39" ht="15">
       <c r="A11" s="107">
         <v>-9.0779999999999993E-3</v>
       </c>
@@ -22215,7 +22216,7 @@
         <v>-8.0649999999999993E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:39" ht="15">
       <c r="A12" s="107">
         <v>-8.6269999999999993E-3</v>
       </c>
@@ -22334,7 +22335,7 @@
         <v>-7.3039999999999997E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:39" ht="15">
       <c r="A13" s="107">
         <v>-7.8659999999999997E-3</v>
       </c>
@@ -22453,7 +22454,7 @@
         <v>-6.5799999999999999E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:39" ht="15">
       <c r="A14" s="107">
         <v>-7.9260000000000008E-3</v>
       </c>
@@ -22572,7 +22573,7 @@
         <v>-6.0819999999999997E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:39" ht="15">
       <c r="A15" s="107">
         <v>-7.7060000000000002E-3</v>
       </c>
@@ -22691,7 +22692,7 @@
         <v>-5.5519999999999996E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:39" ht="15">
       <c r="A16" s="107">
         <v>-7.4400000000000004E-3</v>
       </c>
@@ -22810,7 +22811,7 @@
         <v>-5.1570000000000001E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:39" ht="15">
       <c r="A17" s="107">
         <v>-7.2639999999999996E-3</v>
       </c>
@@ -22929,7 +22930,7 @@
         <v>-4.8859999999999997E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:39" ht="15">
       <c r="A18" s="107">
         <v>-6.6290000000000003E-3</v>
       </c>
@@ -23048,7 +23049,7 @@
         <v>-4.627E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:39" ht="15">
       <c r="A19" s="107">
         <v>-6.1069999999999996E-3</v>
       </c>
@@ -23167,7 +23168,7 @@
         <v>-4.4609999999999997E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:39" ht="15">
       <c r="A20" s="107">
         <v>-6.1700000000000001E-3</v>
       </c>
@@ -23286,7 +23287,7 @@
         <v>-4.2709999999999996E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:39" ht="15">
       <c r="A21" s="107">
         <v>-5.9080000000000001E-3</v>
       </c>
@@ -23405,7 +23406,7 @@
         <v>-4.1130000000000003E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:39" ht="15">
       <c r="A22" s="107">
         <v>-6.0790000000000002E-3</v>
       </c>
@@ -23524,7 +23525,7 @@
         <v>-3.9810000000000002E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:39" ht="15">
       <c r="A23" s="107">
         <v>-6.3879999999999996E-3</v>
       </c>
@@ -23643,7 +23644,7 @@
         <v>-3.7659999999999998E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:39" ht="15">
       <c r="A24" s="107">
         <v>-6.4099999999999999E-3</v>
       </c>
@@ -23762,7 +23763,7 @@
         <v>-3.6419999999999998E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:39" ht="15">
       <c r="A25" s="107">
         <v>-6.496E-3</v>
       </c>
@@ -23881,7 +23882,7 @@
         <v>-3.5969999999999999E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:39" ht="15">
       <c r="A26" s="107">
         <v>-6.483E-3</v>
       </c>
@@ -24000,7 +24001,7 @@
         <v>-3.5360000000000001E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:39" ht="15">
       <c r="A27" s="107">
         <v>-6.4359999999999999E-3</v>
       </c>
@@ -24119,7 +24120,7 @@
         <v>-3.5820000000000001E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:39" ht="15">
       <c r="A28" s="107">
         <v>-6.7730000000000004E-3</v>
       </c>
@@ -24238,7 +24239,7 @@
         <v>-3.578E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:39" ht="15">
       <c r="A29" s="107">
         <v>-6.9969999999999997E-3</v>
       </c>
@@ -24357,7 +24358,7 @@
         <v>-3.5590000000000001E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:39" ht="15">
       <c r="A30" s="107">
         <v>-6.6680000000000003E-3</v>
       </c>
@@ -24476,7 +24477,7 @@
         <v>-3.627E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:39" ht="15">
       <c r="A31" s="107">
         <v>-6.4910000000000002E-3</v>
       </c>
@@ -24595,7 +24596,7 @@
         <v>-3.7659999999999998E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:39" ht="15">
       <c r="A32" s="107">
         <v>-6.0460000000000002E-3</v>
       </c>
@@ -24714,7 +24715,7 @@
         <v>-3.9249999999999997E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:39" ht="15">
       <c r="A33" s="107">
         <v>-5.8809999999999999E-3</v>
       </c>
@@ -24833,7 +24834,7 @@
         <v>-4.0689999999999997E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:39" ht="15">
       <c r="A34" s="107">
         <v>-5.5799999999999999E-3</v>
       </c>
@@ -24952,7 +24953,7 @@
         <v>-4.1269999999999996E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:39" ht="15">
       <c r="A35" s="107">
         <v>-5.176E-3</v>
       </c>
@@ -25071,7 +25072,7 @@
         <v>-4.0930000000000003E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:39" ht="15">
       <c r="A36" s="107">
         <v>-4.9659999999999999E-3</v>
       </c>
@@ -25190,7 +25191,7 @@
         <v>-3.9370000000000004E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:39" ht="15">
       <c r="A37" s="107">
         <v>-4.6490000000000004E-3</v>
       </c>
@@ -25309,7 +25310,7 @@
         <v>-3.5799999999999998E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:39" ht="15">
       <c r="A38" s="107">
         <v>-4.7679999999999997E-3</v>
       </c>
@@ -25428,7 +25429,7 @@
         <v>-3.0119999999999999E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:39" ht="15">
       <c r="A39" s="107">
         <v>-5.019E-3</v>
       </c>
@@ -25547,7 +25548,7 @@
         <v>-2.3739999999999998E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:39" ht="15">
       <c r="A40" s="107">
         <v>-5.0419999999999996E-3</v>
       </c>
@@ -25666,7 +25667,7 @@
         <v>-1.6980000000000001E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:39" ht="15">
       <c r="A41" s="107">
         <v>-5.3030000000000004E-3</v>
       </c>
@@ -25785,7 +25786,7 @@
         <v>-1.181E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:39" ht="15">
       <c r="A42" s="107">
         <v>-5.6730000000000001E-3</v>
       </c>
@@ -25904,7 +25905,7 @@
         <v>-6.9099999999999999E-4</v>
       </c>
     </row>
-    <row r="43" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:39" ht="15">
       <c r="A43" s="107">
         <v>-5.7780000000000001E-3</v>
       </c>
@@ -26023,7 +26024,7 @@
         <v>-3.7399999999999998E-4</v>
       </c>
     </row>
-    <row r="44" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:39" ht="15">
       <c r="A44" s="107">
         <v>-6.2680000000000001E-3</v>
       </c>
@@ -26142,7 +26143,7 @@
         <v>-3.1399999999999999E-4</v>
       </c>
     </row>
-    <row r="45" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:39" ht="15">
       <c r="A45" s="107">
         <v>-7.476E-3</v>
       </c>
@@ -26261,7 +26262,7 @@
         <v>2.104E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:39" ht="15">
       <c r="A46" s="107">
         <v>-7.5620000000000001E-3</v>
       </c>
@@ -26380,7 +26381,7 @@
         <v>2.3509999999999998E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:39" ht="15">
       <c r="A47" s="107">
         <v>-7.4739999999999997E-3</v>
       </c>
@@ -26499,7 +26500,7 @@
         <v>2.5799999999999998E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:39" ht="15">
       <c r="A48" s="107">
         <v>-7.3680000000000004E-3</v>
       </c>
@@ -26618,7 +26619,7 @@
         <v>2.6670000000000001E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:39" ht="15">
       <c r="A49" s="107">
         <v>-7.2680000000000002E-3</v>
       </c>
@@ -26737,7 +26738,7 @@
         <v>2.7320000000000001E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:39" ht="15">
       <c r="A50" s="107">
         <v>-7.0400000000000003E-3</v>
       </c>
@@ -26856,7 +26857,7 @@
         <v>2.794E-3</v>
       </c>
     </row>
-    <row r="51" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:39" ht="15">
       <c r="A51" s="107">
         <v>-6.9129999999999999E-3</v>
       </c>
@@ -26975,7 +26976,7 @@
         <v>2.699E-3</v>
       </c>
     </row>
-    <row r="52" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:39" ht="15">
       <c r="A52" s="107">
         <v>-6.7450000000000001E-3</v>
       </c>
@@ -27094,7 +27095,7 @@
         <v>2.6610000000000002E-3</v>
       </c>
     </row>
-    <row r="53" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:39" ht="15">
       <c r="A53" s="107">
         <v>-6.6499999999999997E-3</v>
       </c>
@@ -27213,7 +27214,7 @@
         <v>2.578E-3</v>
       </c>
     </row>
-    <row r="54" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:39" ht="15">
       <c r="A54" s="107">
         <v>-6.5259999999999997E-3</v>
       </c>
@@ -27332,7 +27333,7 @@
         <v>2.4710000000000001E-3</v>
       </c>
     </row>
-    <row r="55" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:39" ht="15">
       <c r="A55" s="107">
         <v>-6.319E-3</v>
       </c>
@@ -27451,7 +27452,7 @@
         <v>2.3310000000000002E-3</v>
       </c>
     </row>
-    <row r="56" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:39" ht="15">
       <c r="A56" s="107">
         <v>-6.2449999999999997E-3</v>
       </c>
@@ -27570,7 +27571,7 @@
         <v>2.1949999999999999E-3</v>
       </c>
     </row>
-    <row r="57" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:39" ht="15">
       <c r="A57" s="107">
         <v>-6.1310000000000002E-3</v>
       </c>
@@ -27689,7 +27690,7 @@
         <v>2.0049999999999998E-3</v>
       </c>
     </row>
-    <row r="58" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:39" ht="15">
       <c r="A58" s="107">
         <v>-5.9379999999999997E-3</v>
       </c>
@@ -27808,7 +27809,7 @@
         <v>1.8500000000000001E-3</v>
       </c>
     </row>
-    <row r="59" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:39" ht="15">
       <c r="A59" s="107">
         <v>-5.9890000000000004E-3</v>
       </c>
@@ -27927,7 +27928,7 @@
         <v>1.6739999999999999E-3</v>
       </c>
     </row>
-    <row r="60" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:39" ht="15">
       <c r="A60" s="107">
         <v>-5.8269999999999997E-3</v>
       </c>
@@ -28046,7 +28047,7 @@
         <v>1.4710000000000001E-3</v>
       </c>
     </row>
-    <row r="61" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:39" ht="15">
       <c r="A61" s="107">
         <v>-5.6839999999999998E-3</v>
       </c>
@@ -28165,7 +28166,7 @@
         <v>1.3060000000000001E-3</v>
       </c>
     </row>
-    <row r="62" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:39" ht="15">
       <c r="A62" s="107">
         <v>-5.5669999999999999E-3</v>
       </c>
@@ -28284,7 +28285,7 @@
         <v>1.178E-3</v>
       </c>
     </row>
-    <row r="63" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:39" ht="15">
       <c r="A63" s="107">
         <v>-5.293E-3</v>
       </c>
@@ -28403,7 +28404,7 @@
         <v>9.2299999999999999E-4</v>
       </c>
     </row>
-    <row r="64" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:39" ht="15">
       <c r="A64" s="107">
         <v>-5.1089999999999998E-3</v>
       </c>
@@ -28522,7 +28523,7 @@
         <v>7.2999999999999996E-4</v>
       </c>
     </row>
-    <row r="65" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:39" ht="15">
       <c r="A65" s="107">
         <v>-4.849E-3</v>
       </c>
@@ -28641,7 +28642,7 @@
         <v>4.4900000000000002E-4</v>
       </c>
     </row>
-    <row r="66" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:39" ht="15">
       <c r="A66" s="107">
         <v>-4.3210000000000002E-3</v>
       </c>
@@ -28760,7 +28761,7 @@
         <v>2.52E-4</v>
       </c>
     </row>
-    <row r="67" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:39" ht="15">
       <c r="A67" s="107">
         <v>-4.4910000000000002E-3</v>
       </c>
@@ -28879,7 +28880,7 @@
         <v>4.1999999999999998E-5</v>
       </c>
     </row>
-    <row r="68" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:39" ht="15">
       <c r="A68" s="107">
         <v>-4.2199999999999998E-3</v>
       </c>
@@ -28998,7 +28999,7 @@
         <v>-1.84E-4</v>
       </c>
     </row>
-    <row r="69" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:39" ht="15">
       <c r="A69" s="107">
         <v>-4.0210000000000003E-3</v>
       </c>
@@ -29117,7 +29118,7 @@
         <v>-4.3899999999999999E-4</v>
       </c>
     </row>
-    <row r="70" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:39" ht="15">
       <c r="A70" s="107">
         <v>-3.8509999999999998E-3</v>
       </c>
@@ -29236,7 +29237,7 @@
         <v>-5.9400000000000002E-4</v>
       </c>
     </row>
-    <row r="71" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:39" ht="15">
       <c r="A71" s="107">
         <v>-3.5309999999999999E-3</v>
       </c>
@@ -29355,7 +29356,7 @@
         <v>-7.4600000000000003E-4</v>
       </c>
     </row>
-    <row r="72" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:39" ht="15">
       <c r="A72" s="107">
         <v>-3.3899999999999998E-3</v>
       </c>
@@ -29474,7 +29475,7 @@
         <v>-8.0599999999999997E-4</v>
       </c>
     </row>
-    <row r="73" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:39" ht="15">
       <c r="A73" s="107">
         <v>-3.284E-3</v>
       </c>
@@ -29593,7 +29594,7 @@
         <v>-7.0600000000000003E-4</v>
       </c>
     </row>
-    <row r="74" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:39" ht="15">
       <c r="A74" s="107">
         <v>-3.0469999999999998E-3</v>
       </c>
@@ -29712,7 +29713,7 @@
         <v>-5.2499999999999997E-4</v>
       </c>
     </row>
-    <row r="75" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:39" ht="15">
       <c r="A75" s="107">
         <v>-3.068E-3</v>
       </c>
@@ -29831,7 +29832,7 @@
         <v>-2.22E-4</v>
       </c>
     </row>
-    <row r="76" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:39" ht="15">
       <c r="A76" s="107">
         <v>-3.1979999999999999E-3</v>
       </c>
@@ -29950,7 +29951,7 @@
         <v>2.02E-4</v>
       </c>
     </row>
-    <row r="77" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:39" ht="15">
       <c r="A77" s="107">
         <v>-3.3509999999999998E-3</v>
       </c>
@@ -30069,7 +30070,7 @@
         <v>6.6100000000000002E-4</v>
       </c>
     </row>
-    <row r="78" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:39" ht="15">
       <c r="A78" s="107">
         <v>-3.565E-3</v>
       </c>
@@ -30188,7 +30189,7 @@
         <v>1.021E-3</v>
       </c>
     </row>
-    <row r="79" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:39" ht="15">
       <c r="A79" s="107">
         <v>-3.4989999999999999E-3</v>
       </c>
@@ -30307,7 +30308,7 @@
         <v>1.351E-3</v>
       </c>
     </row>
-    <row r="80" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:39" ht="15">
       <c r="A80" s="107">
         <v>-3.6089999999999998E-3</v>
       </c>
@@ -30426,7 +30427,7 @@
         <v>1.5250000000000001E-3</v>
       </c>
     </row>
-    <row r="81" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:39" ht="15">
       <c r="A81" s="107">
         <v>-3.872E-3</v>
       </c>
@@ -30545,7 +30546,7 @@
         <v>1.536E-3</v>
       </c>
     </row>
-    <row r="82" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:39" ht="15">
       <c r="A82" s="107">
         <v>-3.9810000000000002E-3</v>
       </c>
@@ -30664,7 +30665,7 @@
         <v>1.41E-3</v>
       </c>
     </row>
-    <row r="83" spans="1:39" ht="15" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:39" ht="15">
       <c r="A83" s="107">
         <v>-5.2859999999999999E-3</v>
       </c>

</xml_diff>